<commit_message>
Auto push 2023-04-20 18:13:57.81
</commit_message>
<xml_diff>
--- a/note/10_2ndTeamProject/일정관리.xlsx
+++ b/note/10_2ndTeamProject/일정관리.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\이전수업자료\1_웹PG\note\10_2nd TEAM Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\webPro\note\10_2ndTeamProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="8595" windowHeight="11730"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="8595" windowHeight="11730" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="4" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="Sheet1" sheetId="8" r:id="rId5"/>
     <sheet name="팀구성" sheetId="9" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="352">
   <si>
     <t>이용자 권한과 기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1430,19 +1430,118 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>강동주, 김한울, 윤여송</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>강성빈, 김성연, 김훈, 안중권</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>김소연, 신치윤, 유민상</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>김혜린, 임동은, 진윤진</t>
+    <t>스터디모집</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="25"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>강동주</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="25"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 김한울, 윤여송</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제주도 홍보</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">강성빈, 김성연, 김훈, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="25"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>안중권</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>애견 용품 쇼핑몰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">김소연, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="25"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>신치윤</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="25"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 유민상</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>놀이동산</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="25"/>
+        <color rgb="FF0000FF"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>김혜린</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="25"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 임동은, 진윤진</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1450,7 +1549,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1582,6 +1681,15 @@
     <font>
       <sz val="25"/>
       <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="25"/>
+      <color rgb="FF0000FF"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -2371,6 +2479,42 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -2389,94 +2533,73 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="25" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="25" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2497,34 +2620,25 @@
     <xf numFmtId="0" fontId="12" fillId="25" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2552,12 +2666,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2596,6 +2704,7 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FF0000FF"/>
       <color rgb="FFFFFFCC"/>
       <color rgb="FFFFFFFF"/>
       <color rgb="FFE1FFE1"/>
@@ -2605,7 +2714,6 @@
       <color rgb="FFE5F4F7"/>
       <color rgb="FFCCFFCC"/>
       <color rgb="FFCCFFFF"/>
-      <color rgb="FFFFFF99"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2908,7 +3016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AD22" sqref="AD22"/>
     </sheetView>
   </sheetViews>
@@ -2926,61 +3034,61 @@
     <row r="1" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="94" t="s">
         <v>340</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="83"/>
-      <c r="O2" s="83"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="83"/>
-      <c r="R2" s="83"/>
-      <c r="S2" s="83"/>
-      <c r="T2" s="83"/>
-      <c r="U2" s="83"/>
-      <c r="V2" s="83"/>
-      <c r="W2" s="83"/>
-      <c r="X2" s="83"/>
-      <c r="Y2" s="83"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="95"/>
+      <c r="J2" s="95"/>
+      <c r="K2" s="95"/>
+      <c r="L2" s="95"/>
+      <c r="M2" s="95"/>
+      <c r="N2" s="95"/>
+      <c r="O2" s="95"/>
+      <c r="P2" s="95"/>
+      <c r="Q2" s="95"/>
+      <c r="R2" s="95"/>
+      <c r="S2" s="95"/>
+      <c r="T2" s="95"/>
+      <c r="U2" s="95"/>
+      <c r="V2" s="95"/>
+      <c r="W2" s="95"/>
+      <c r="X2" s="95"/>
+      <c r="Y2" s="95"/>
       <c r="Z2" s="5"/>
       <c r="AA2" s="5"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="83"/>
-      <c r="C3" s="83"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
-      <c r="I3" s="83"/>
-      <c r="J3" s="83"/>
-      <c r="K3" s="83"/>
-      <c r="L3" s="83"/>
-      <c r="M3" s="83"/>
-      <c r="N3" s="83"/>
-      <c r="O3" s="83"/>
-      <c r="P3" s="83"/>
-      <c r="Q3" s="83"/>
-      <c r="R3" s="83"/>
-      <c r="S3" s="83"/>
-      <c r="T3" s="83"/>
-      <c r="U3" s="83"/>
-      <c r="V3" s="83"/>
-      <c r="W3" s="83"/>
-      <c r="X3" s="83"/>
-      <c r="Y3" s="83"/>
+      <c r="B3" s="95"/>
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+      <c r="I3" s="95"/>
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95"/>
+      <c r="O3" s="95"/>
+      <c r="P3" s="95"/>
+      <c r="Q3" s="95"/>
+      <c r="R3" s="95"/>
+      <c r="S3" s="95"/>
+      <c r="T3" s="95"/>
+      <c r="U3" s="95"/>
+      <c r="V3" s="95"/>
+      <c r="W3" s="95"/>
+      <c r="X3" s="95"/>
+      <c r="Y3" s="95"/>
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
     </row>
@@ -3045,44 +3153,44 @@
     <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
       <c r="B6" s="22"/>
-      <c r="C6" s="84" t="s">
+      <c r="C6" s="96" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="23"/>
-      <c r="E6" s="86" t="s">
+      <c r="E6" s="83" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="86"/>
-      <c r="J6" s="86"/>
-      <c r="K6" s="87"/>
-      <c r="L6" s="93" t="s">
+      <c r="F6" s="83"/>
+      <c r="G6" s="83"/>
+      <c r="H6" s="83"/>
+      <c r="I6" s="83"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="84"/>
+      <c r="L6" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="86"/>
-      <c r="N6" s="86"/>
-      <c r="O6" s="86"/>
-      <c r="P6" s="86"/>
-      <c r="Q6" s="86"/>
-      <c r="R6" s="87"/>
-      <c r="S6" s="93" t="s">
+      <c r="M6" s="83"/>
+      <c r="N6" s="83"/>
+      <c r="O6" s="83"/>
+      <c r="P6" s="83"/>
+      <c r="Q6" s="83"/>
+      <c r="R6" s="84"/>
+      <c r="S6" s="82" t="s">
         <v>185</v>
       </c>
-      <c r="T6" s="86"/>
-      <c r="U6" s="86"/>
-      <c r="V6" s="86"/>
-      <c r="W6" s="86"/>
-      <c r="X6" s="86"/>
-      <c r="Y6" s="86"/>
+      <c r="T6" s="83"/>
+      <c r="U6" s="83"/>
+      <c r="V6" s="83"/>
+      <c r="W6" s="83"/>
+      <c r="X6" s="83"/>
+      <c r="Y6" s="83"/>
       <c r="Z6" s="24"/>
       <c r="AA6" s="5"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
       <c r="B7" s="15"/>
-      <c r="C7" s="85"/>
+      <c r="C7" s="97"/>
       <c r="D7" s="25"/>
       <c r="E7" s="15">
         <v>13</v>
@@ -3238,7 +3346,7 @@
     <row r="11" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="88" t="s">
+      <c r="C11" s="98" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="42"/>
@@ -3269,7 +3377,7 @@
     <row r="12" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="88"/>
+      <c r="C12" s="98"/>
       <c r="D12" s="41"/>
       <c r="E12" s="8"/>
       <c r="F12" s="6"/>
@@ -3327,7 +3435,7 @@
     <row r="14" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="90" t="s">
+      <c r="C14" s="99" t="s">
         <v>44</v>
       </c>
       <c r="D14" s="11"/>
@@ -3358,7 +3466,7 @@
     <row r="15" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="90"/>
+      <c r="C15" s="99"/>
       <c r="D15" s="11"/>
       <c r="E15" s="8"/>
       <c r="F15" s="6"/>
@@ -3416,7 +3524,7 @@
     <row r="17" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="88" t="s">
+      <c r="C17" s="98" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="10"/>
@@ -3447,7 +3555,7 @@
     <row r="18" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="88"/>
+      <c r="C18" s="98"/>
       <c r="D18" s="10"/>
       <c r="E18" s="6"/>
       <c r="F18" s="8"/>
@@ -3536,7 +3644,7 @@
     <row r="21" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
       <c r="B21" s="6"/>
-      <c r="C21" s="89" t="s">
+      <c r="C21" s="91" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="12"/>
@@ -3567,7 +3675,7 @@
     <row r="22" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="89"/>
+      <c r="C22" s="91"/>
       <c r="D22" s="12"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
@@ -3625,7 +3733,7 @@
     <row r="24" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="18"/>
       <c r="B24" s="6"/>
-      <c r="C24" s="89" t="s">
+      <c r="C24" s="91" t="s">
         <v>31</v>
       </c>
       <c r="D24" s="12"/>
@@ -3656,7 +3764,7 @@
     <row r="25" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18"/>
       <c r="B25" s="6"/>
-      <c r="C25" s="89"/>
+      <c r="C25" s="91"/>
       <c r="D25" s="12"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
@@ -3714,7 +3822,7 @@
     <row r="27" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
       <c r="B27" s="6"/>
-      <c r="C27" s="89" t="s">
+      <c r="C27" s="91" t="s">
         <v>27</v>
       </c>
       <c r="D27" s="12"/>
@@ -3745,7 +3853,7 @@
     <row r="28" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18"/>
       <c r="B28" s="6"/>
-      <c r="C28" s="89"/>
+      <c r="C28" s="91"/>
       <c r="D28" s="12"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
@@ -3803,7 +3911,7 @@
     <row r="30" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18"/>
       <c r="B30" s="6"/>
-      <c r="C30" s="89" t="s">
+      <c r="C30" s="91" t="s">
         <v>28</v>
       </c>
       <c r="D30" s="12"/>
@@ -3834,7 +3942,7 @@
     <row r="31" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="89"/>
+      <c r="C31" s="91"/>
       <c r="D31" s="12"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
@@ -3892,7 +4000,7 @@
     <row r="33" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="18"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="89" t="s">
+      <c r="C33" s="91" t="s">
         <v>26</v>
       </c>
       <c r="D33" s="12"/>
@@ -3923,7 +4031,7 @@
     <row r="34" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="18"/>
       <c r="B34" s="6"/>
-      <c r="C34" s="89"/>
+      <c r="C34" s="91"/>
       <c r="D34" s="12"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -3981,7 +4089,7 @@
     <row r="36" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="18"/>
       <c r="B36" s="6"/>
-      <c r="C36" s="89" t="s">
+      <c r="C36" s="91" t="s">
         <v>42</v>
       </c>
       <c r="D36" s="12"/>
@@ -4012,7 +4120,7 @@
     <row r="37" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="18"/>
       <c r="B37" s="6"/>
-      <c r="C37" s="89"/>
+      <c r="C37" s="91"/>
       <c r="D37" s="12"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
@@ -4101,7 +4209,7 @@
     <row r="40" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="18"/>
       <c r="B40" s="6"/>
-      <c r="C40" s="80" t="s">
+      <c r="C40" s="92" t="s">
         <v>30</v>
       </c>
       <c r="D40" s="12"/>
@@ -4132,7 +4240,7 @@
     <row r="41" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="80"/>
+      <c r="C41" s="92"/>
       <c r="D41" s="12"/>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
@@ -4190,7 +4298,7 @@
     <row r="43" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18"/>
       <c r="B43" s="6"/>
-      <c r="C43" s="80" t="s">
+      <c r="C43" s="92" t="s">
         <v>29</v>
       </c>
       <c r="D43" s="12"/>
@@ -4221,7 +4329,7 @@
     <row r="44" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="18"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="80"/>
+      <c r="C44" s="92"/>
       <c r="D44" s="12"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
@@ -4279,7 +4387,7 @@
     <row r="46" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="18"/>
       <c r="B46" s="6"/>
-      <c r="C46" s="80" t="s">
+      <c r="C46" s="92" t="s">
         <v>2</v>
       </c>
       <c r="D46" s="12"/>
@@ -4310,7 +4418,7 @@
     <row r="47" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="80"/>
+      <c r="C47" s="92"/>
       <c r="D47" s="12"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
@@ -4368,7 +4476,7 @@
     <row r="49" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="18"/>
       <c r="B49" s="6"/>
-      <c r="C49" s="80" t="s">
+      <c r="C49" s="92" t="s">
         <v>37</v>
       </c>
       <c r="D49" s="12"/>
@@ -4399,7 +4507,7 @@
     <row r="50" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="18"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="80"/>
+      <c r="C50" s="92"/>
       <c r="D50" s="12"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
@@ -4488,7 +4596,7 @@
     <row r="53" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="18"/>
       <c r="B53" s="6"/>
-      <c r="C53" s="91" t="s">
+      <c r="C53" s="81" t="s">
         <v>32</v>
       </c>
       <c r="D53" s="10"/>
@@ -4519,7 +4627,7 @@
     <row r="54" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="18"/>
       <c r="B54" s="6"/>
-      <c r="C54" s="91"/>
+      <c r="C54" s="81"/>
       <c r="D54" s="10"/>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
@@ -4577,7 +4685,7 @@
     <row r="56" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="18"/>
       <c r="B56" s="6"/>
-      <c r="C56" s="91" t="s">
+      <c r="C56" s="81" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10"/>
@@ -4608,7 +4716,7 @@
     <row r="57" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="18"/>
       <c r="B57" s="6"/>
-      <c r="C57" s="91"/>
+      <c r="C57" s="81"/>
       <c r="D57" s="10"/>
       <c r="E57" s="6"/>
       <c r="F57" s="6"/>
@@ -4666,7 +4774,7 @@
     <row r="59" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="18"/>
       <c r="B59" s="6"/>
-      <c r="C59" s="91" t="s">
+      <c r="C59" s="81" t="s">
         <v>34</v>
       </c>
       <c r="D59" s="10"/>
@@ -4697,7 +4805,7 @@
     <row r="60" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="18"/>
       <c r="B60" s="6"/>
-      <c r="C60" s="91"/>
+      <c r="C60" s="81"/>
       <c r="D60" s="10"/>
       <c r="E60" s="6"/>
       <c r="F60" s="6"/>
@@ -4755,7 +4863,7 @@
     <row r="62" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="18"/>
       <c r="B62" s="6"/>
-      <c r="C62" s="91" t="s">
+      <c r="C62" s="81" t="s">
         <v>35</v>
       </c>
       <c r="D62" s="10"/>
@@ -4786,7 +4894,7 @@
     <row r="63" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="18"/>
       <c r="B63" s="6"/>
-      <c r="C63" s="91"/>
+      <c r="C63" s="81"/>
       <c r="D63" s="10"/>
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
@@ -4844,7 +4952,7 @@
     <row r="65" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="18"/>
       <c r="B65" s="6"/>
-      <c r="C65" s="91" t="s">
+      <c r="C65" s="81" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="12"/>
@@ -4875,7 +4983,7 @@
     <row r="66" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="18"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="91"/>
+      <c r="C66" s="81"/>
       <c r="D66" s="12"/>
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
@@ -4933,7 +5041,7 @@
     <row r="68" spans="1:27" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="18"/>
       <c r="B68" s="6"/>
-      <c r="C68" s="81" t="s">
+      <c r="C68" s="93" t="s">
         <v>167</v>
       </c>
       <c r="D68" s="7"/>
@@ -4964,7 +5072,7 @@
     <row r="69" spans="1:27" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="18"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="81"/>
+      <c r="C69" s="93"/>
       <c r="D69" s="7"/>
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
@@ -5053,40 +5161,40 @@
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
-      <c r="E72" s="92" t="s">
+      <c r="E72" s="80" t="s">
         <v>186</v>
       </c>
-      <c r="F72" s="92"/>
+      <c r="F72" s="80"/>
       <c r="G72" s="58"/>
-      <c r="H72" s="99" t="s">
+      <c r="H72" s="90" t="s">
         <v>184</v>
       </c>
-      <c r="I72" s="99"/>
+      <c r="I72" s="90"/>
       <c r="J72" s="57"/>
-      <c r="K72" s="98" t="s">
+      <c r="K72" s="89" t="s">
         <v>183</v>
       </c>
-      <c r="L72" s="98"/>
+      <c r="L72" s="89"/>
       <c r="M72" s="57"/>
-      <c r="N72" s="97" t="s">
+      <c r="N72" s="88" t="s">
         <v>182</v>
       </c>
-      <c r="O72" s="97"/>
+      <c r="O72" s="88"/>
       <c r="P72" s="57"/>
-      <c r="Q72" s="96" t="s">
+      <c r="Q72" s="87" t="s">
         <v>181</v>
       </c>
-      <c r="R72" s="96"/>
+      <c r="R72" s="87"/>
       <c r="S72" s="57"/>
-      <c r="T72" s="95" t="s">
+      <c r="T72" s="86" t="s">
         <v>180</v>
       </c>
-      <c r="U72" s="95"/>
+      <c r="U72" s="86"/>
       <c r="V72" s="57"/>
-      <c r="W72" s="94" t="s">
+      <c r="W72" s="85" t="s">
         <v>179</v>
       </c>
-      <c r="X72" s="94"/>
+      <c r="X72" s="85"/>
       <c r="Y72" s="5"/>
       <c r="Z72" s="5"/>
       <c r="AA72" s="5"/>
@@ -5121,6 +5229,21 @@
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="B2:Y3"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E6:K6"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C46:C47"/>
     <mergeCell ref="E72:F72"/>
     <mergeCell ref="C59:C60"/>
     <mergeCell ref="C62:C63"/>
@@ -5137,21 +5260,6 @@
     <mergeCell ref="C53:C54"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C43:C44"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="B2:Y3"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="E6:K6"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C46:C47"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5461,25 +5569,25 @@
       <c r="N2" s="59"/>
     </row>
     <row r="3" spans="2:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="123" t="s">
+      <c r="B3" s="105" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="123" t="s">
+      <c r="C3" s="105" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="113" t="s">
+      <c r="D3" s="114" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="113" t="s">
+      <c r="E3" s="114" t="s">
         <v>59</v>
       </c>
       <c r="F3" s="65" t="s">
         <v>273</v>
       </c>
-      <c r="G3" s="113" t="s">
+      <c r="G3" s="114" t="s">
         <v>249</v>
       </c>
-      <c r="H3" s="113" t="s">
+      <c r="H3" s="114" t="s">
         <v>250</v>
       </c>
       <c r="I3" s="65" t="s">
@@ -5497,15 +5605,15 @@
       <c r="O3" s="59"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="126"/>
-      <c r="C4" s="126"/>
+      <c r="B4" s="106"/>
+      <c r="C4" s="106"/>
       <c r="D4" s="115"/>
       <c r="E4" s="115"/>
       <c r="F4" s="65" t="s">
         <v>275</v>
       </c>
-      <c r="G4" s="114"/>
-      <c r="H4" s="114"/>
+      <c r="G4" s="116"/>
+      <c r="H4" s="116"/>
       <c r="I4" s="65" t="s">
         <v>171</v>
       </c>
@@ -5523,19 +5631,19 @@
       <c r="O4" s="59"/>
     </row>
     <row r="5" spans="2:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="126"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="113" t="s">
+      <c r="B5" s="106"/>
+      <c r="C5" s="106"/>
+      <c r="D5" s="114" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="113" t="s">
+      <c r="E5" s="114" t="s">
         <v>56</v>
       </c>
       <c r="F5" s="65" t="s">
         <v>274</v>
       </c>
-      <c r="G5" s="114"/>
-      <c r="H5" s="114"/>
+      <c r="G5" s="116"/>
+      <c r="H5" s="116"/>
       <c r="I5" s="65"/>
       <c r="J5" s="65"/>
       <c r="K5" s="65" t="s">
@@ -5549,15 +5657,15 @@
       <c r="O5" s="59"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="126"/>
-      <c r="C6" s="126"/>
+      <c r="B6" s="106"/>
+      <c r="C6" s="106"/>
       <c r="D6" s="115"/>
       <c r="E6" s="115"/>
       <c r="F6" s="65" t="s">
         <v>276</v>
       </c>
-      <c r="G6" s="114"/>
-      <c r="H6" s="114"/>
+      <c r="G6" s="116"/>
+      <c r="H6" s="116"/>
       <c r="I6" s="65" t="s">
         <v>169</v>
       </c>
@@ -5575,19 +5683,19 @@
       <c r="O6" s="59"/>
     </row>
     <row r="7" spans="2:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="126"/>
-      <c r="C7" s="126"/>
-      <c r="D7" s="113" t="s">
+      <c r="B7" s="106"/>
+      <c r="C7" s="106"/>
+      <c r="D7" s="114" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="116" t="s">
+      <c r="E7" s="121" t="s">
         <v>94</v>
       </c>
       <c r="F7" s="65" t="s">
         <v>278</v>
       </c>
-      <c r="G7" s="114"/>
-      <c r="H7" s="114"/>
+      <c r="G7" s="116"/>
+      <c r="H7" s="116"/>
       <c r="I7" s="65" t="s">
         <v>172</v>
       </c>
@@ -5603,15 +5711,15 @@
       <c r="O7" s="59"/>
     </row>
     <row r="8" spans="2:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="126"/>
-      <c r="C8" s="126"/>
-      <c r="D8" s="114"/>
-      <c r="E8" s="117"/>
+      <c r="B8" s="106"/>
+      <c r="C8" s="106"/>
+      <c r="D8" s="116"/>
+      <c r="E8" s="122"/>
       <c r="F8" s="65" t="s">
         <v>277</v>
       </c>
-      <c r="G8" s="114"/>
-      <c r="H8" s="114"/>
+      <c r="G8" s="116"/>
+      <c r="H8" s="116"/>
       <c r="I8" s="65" t="s">
         <v>173</v>
       </c>
@@ -5627,10 +5735,10 @@
       <c r="O8" s="59"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="127"/>
-      <c r="C9" s="127"/>
+      <c r="B9" s="107"/>
+      <c r="C9" s="107"/>
       <c r="D9" s="115"/>
-      <c r="E9" s="118"/>
+      <c r="E9" s="123"/>
       <c r="F9" s="65" t="s">
         <v>279</v>
       </c>
@@ -5647,25 +5755,25 @@
       <c r="O9" s="59"/>
     </row>
     <row r="10" spans="2:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="124" t="s">
+      <c r="B10" s="108" t="s">
         <v>166</v>
       </c>
-      <c r="C10" s="123" t="s">
+      <c r="C10" s="105" t="s">
         <v>165</v>
       </c>
-      <c r="D10" s="130" t="s">
+      <c r="D10" s="117" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="110" t="s">
+      <c r="E10" s="102" t="s">
         <v>70</v>
       </c>
       <c r="F10" s="47" t="s">
         <v>282</v>
       </c>
-      <c r="G10" s="110" t="s">
+      <c r="G10" s="102" t="s">
         <v>251</v>
       </c>
-      <c r="H10" s="110" t="s">
+      <c r="H10" s="102" t="s">
         <v>252</v>
       </c>
       <c r="I10" s="47"/>
@@ -5679,15 +5787,15 @@
       <c r="O10" s="59"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="124"/>
-      <c r="C11" s="126"/>
-      <c r="D11" s="130"/>
-      <c r="E11" s="112"/>
+      <c r="B11" s="108"/>
+      <c r="C11" s="106"/>
+      <c r="D11" s="117"/>
+      <c r="E11" s="103"/>
       <c r="F11" s="47" t="s">
         <v>281</v>
       </c>
-      <c r="G11" s="111"/>
-      <c r="H11" s="111"/>
+      <c r="G11" s="118"/>
+      <c r="H11" s="118"/>
       <c r="I11" s="47"/>
       <c r="J11" s="47" t="s">
         <v>79</v>
@@ -5699,8 +5807,8 @@
       <c r="O11" s="59"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="124"/>
-      <c r="C12" s="126"/>
+      <c r="B12" s="108"/>
+      <c r="C12" s="106"/>
       <c r="D12" s="47" t="s">
         <v>75</v>
       </c>
@@ -5710,8 +5818,8 @@
       <c r="F12" s="47" t="s">
         <v>280</v>
       </c>
-      <c r="G12" s="111"/>
-      <c r="H12" s="111"/>
+      <c r="G12" s="118"/>
+      <c r="H12" s="118"/>
       <c r="I12" s="47"/>
       <c r="J12" s="47" t="s">
         <v>157</v>
@@ -5725,19 +5833,19 @@
       <c r="O12" s="59"/>
     </row>
     <row r="13" spans="2:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="124"/>
-      <c r="C13" s="126"/>
-      <c r="D13" s="110" t="s">
+      <c r="B13" s="108"/>
+      <c r="C13" s="106"/>
+      <c r="D13" s="102" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="110" t="s">
+      <c r="E13" s="102" t="s">
         <v>73</v>
       </c>
       <c r="F13" s="47" t="s">
         <v>283</v>
       </c>
-      <c r="G13" s="111"/>
-      <c r="H13" s="111"/>
+      <c r="G13" s="118"/>
+      <c r="H13" s="118"/>
       <c r="I13" s="47"/>
       <c r="J13" s="47" t="s">
         <v>157</v>
@@ -5751,15 +5859,15 @@
       <c r="O13" s="59"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14" s="124"/>
-      <c r="C14" s="126"/>
-      <c r="D14" s="112"/>
-      <c r="E14" s="112"/>
+      <c r="B14" s="108"/>
+      <c r="C14" s="106"/>
+      <c r="D14" s="103"/>
+      <c r="E14" s="103"/>
       <c r="F14" s="72" t="s">
         <v>284</v>
       </c>
-      <c r="G14" s="111"/>
-      <c r="H14" s="111"/>
+      <c r="G14" s="118"/>
+      <c r="H14" s="118"/>
       <c r="I14" s="47"/>
       <c r="J14" s="47" t="s">
         <v>79</v>
@@ -5773,8 +5881,8 @@
       <c r="O14" s="59"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B15" s="124"/>
-      <c r="C15" s="127"/>
+      <c r="B15" s="108"/>
+      <c r="C15" s="107"/>
       <c r="D15" s="47" t="s">
         <v>71</v>
       </c>
@@ -5784,8 +5892,8 @@
       <c r="F15" s="47" t="s">
         <v>285</v>
       </c>
-      <c r="G15" s="112"/>
-      <c r="H15" s="112"/>
+      <c r="G15" s="103"/>
+      <c r="H15" s="103"/>
       <c r="I15" s="47"/>
       <c r="J15" s="47" t="s">
         <v>157</v>
@@ -5797,23 +5905,23 @@
       <c r="O15" s="59"/>
     </row>
     <row r="16" spans="2:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="124"/>
-      <c r="C16" s="128" t="s">
+      <c r="B16" s="108"/>
+      <c r="C16" s="104" t="s">
         <v>101</v>
       </c>
-      <c r="D16" s="131" t="s">
+      <c r="D16" s="101" t="s">
         <v>83</v>
       </c>
-      <c r="E16" s="104" t="s">
+      <c r="E16" s="119" t="s">
         <v>86</v>
       </c>
       <c r="F16" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="G16" s="104" t="s">
+      <c r="G16" s="119" t="s">
         <v>253</v>
       </c>
-      <c r="H16" s="104" t="s">
+      <c r="H16" s="119" t="s">
         <v>254</v>
       </c>
       <c r="I16" s="49"/>
@@ -5827,15 +5935,15 @@
       <c r="O16" s="59"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B17" s="124"/>
-      <c r="C17" s="128"/>
-      <c r="D17" s="131"/>
-      <c r="E17" s="106"/>
+      <c r="B17" s="108"/>
+      <c r="C17" s="104"/>
+      <c r="D17" s="101"/>
+      <c r="E17" s="120"/>
       <c r="F17" s="70" t="s">
         <v>287</v>
       </c>
-      <c r="G17" s="105"/>
-      <c r="H17" s="105"/>
+      <c r="G17" s="128"/>
+      <c r="H17" s="128"/>
       <c r="I17" s="49"/>
       <c r="J17" s="49" t="s">
         <v>85</v>
@@ -5847,8 +5955,8 @@
       <c r="O17" s="59"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B18" s="124"/>
-      <c r="C18" s="128"/>
+      <c r="B18" s="108"/>
+      <c r="C18" s="104"/>
       <c r="D18" s="49" t="s">
         <v>87</v>
       </c>
@@ -5858,8 +5966,8 @@
       <c r="F18" s="49" t="s">
         <v>288</v>
       </c>
-      <c r="G18" s="105"/>
-      <c r="H18" s="105"/>
+      <c r="G18" s="128"/>
+      <c r="H18" s="128"/>
       <c r="I18" s="49"/>
       <c r="J18" s="49"/>
       <c r="K18" s="49" t="s">
@@ -5871,8 +5979,8 @@
       <c r="O18" s="59"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B19" s="124"/>
-      <c r="C19" s="128"/>
+      <c r="B19" s="108"/>
+      <c r="C19" s="104"/>
       <c r="D19" s="49" t="s">
         <v>88</v>
       </c>
@@ -5882,8 +5990,8 @@
       <c r="F19" s="49" t="s">
         <v>289</v>
       </c>
-      <c r="G19" s="105"/>
-      <c r="H19" s="105"/>
+      <c r="G19" s="128"/>
+      <c r="H19" s="128"/>
       <c r="I19" s="49"/>
       <c r="J19" s="49" t="s">
         <v>155</v>
@@ -5897,19 +6005,19 @@
       <c r="O19" s="59"/>
     </row>
     <row r="20" spans="2:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="124"/>
-      <c r="C20" s="128"/>
-      <c r="D20" s="131" t="s">
+      <c r="B20" s="108"/>
+      <c r="C20" s="104"/>
+      <c r="D20" s="101" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="104" t="s">
+      <c r="E20" s="119" t="s">
         <v>96</v>
       </c>
       <c r="F20" s="49" t="s">
         <v>290</v>
       </c>
-      <c r="G20" s="105"/>
-      <c r="H20" s="105"/>
+      <c r="G20" s="128"/>
+      <c r="H20" s="128"/>
       <c r="I20" s="49"/>
       <c r="J20" s="49" t="s">
         <v>155</v>
@@ -5923,15 +6031,15 @@
       <c r="O20" s="59"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B21" s="124"/>
-      <c r="C21" s="128"/>
-      <c r="D21" s="131"/>
-      <c r="E21" s="106"/>
+      <c r="B21" s="108"/>
+      <c r="C21" s="104"/>
+      <c r="D21" s="101"/>
+      <c r="E21" s="120"/>
       <c r="F21" s="70" t="s">
         <v>291</v>
       </c>
-      <c r="G21" s="105"/>
-      <c r="H21" s="105"/>
+      <c r="G21" s="128"/>
+      <c r="H21" s="128"/>
       <c r="I21" s="49"/>
       <c r="J21" s="49" t="s">
         <v>85</v>
@@ -5943,8 +6051,8 @@
       <c r="O21" s="59"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B22" s="125"/>
-      <c r="C22" s="128"/>
+      <c r="B22" s="109"/>
+      <c r="C22" s="104"/>
       <c r="D22" s="49" t="s">
         <v>90</v>
       </c>
@@ -5954,8 +6062,8 @@
       <c r="F22" s="49" t="s">
         <v>292</v>
       </c>
-      <c r="G22" s="106"/>
-      <c r="H22" s="106"/>
+      <c r="G22" s="120"/>
+      <c r="H22" s="120"/>
       <c r="I22" s="49"/>
       <c r="J22" s="49" t="s">
         <v>155</v>
@@ -5967,10 +6075,10 @@
       <c r="O22" s="59"/>
     </row>
     <row r="23" spans="2:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="128" t="s">
+      <c r="B23" s="104" t="s">
         <v>136</v>
       </c>
-      <c r="C23" s="128" t="s">
+      <c r="C23" s="104" t="s">
         <v>112</v>
       </c>
       <c r="D23" s="48" t="s">
@@ -5982,10 +6090,10 @@
       <c r="F23" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="G23" s="107" t="s">
+      <c r="G23" s="129" t="s">
         <v>294</v>
       </c>
-      <c r="H23" s="107" t="s">
+      <c r="H23" s="129" t="s">
         <v>295</v>
       </c>
       <c r="I23" s="48"/>
@@ -5999,8 +6107,8 @@
       <c r="O23" s="59"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B24" s="129"/>
-      <c r="C24" s="128"/>
+      <c r="B24" s="111"/>
+      <c r="C24" s="104"/>
       <c r="D24" s="48" t="s">
         <v>109</v>
       </c>
@@ -6010,8 +6118,8 @@
       <c r="F24" s="48" t="s">
         <v>296</v>
       </c>
-      <c r="G24" s="108"/>
-      <c r="H24" s="108"/>
+      <c r="G24" s="130"/>
+      <c r="H24" s="130"/>
       <c r="I24" s="48"/>
       <c r="J24" s="48" t="s">
         <v>60</v>
@@ -6025,8 +6133,8 @@
       <c r="O24" s="59"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B25" s="129"/>
-      <c r="C25" s="128"/>
+      <c r="B25" s="111"/>
+      <c r="C25" s="104"/>
       <c r="D25" s="48" t="s">
         <v>110</v>
       </c>
@@ -6036,8 +6144,8 @@
       <c r="F25" s="48" t="s">
         <v>297</v>
       </c>
-      <c r="G25" s="108"/>
-      <c r="H25" s="108"/>
+      <c r="G25" s="130"/>
+      <c r="H25" s="130"/>
       <c r="I25" s="48"/>
       <c r="J25" s="48"/>
       <c r="K25" s="48" t="s">
@@ -6049,8 +6157,8 @@
       <c r="O25" s="59"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B26" s="129"/>
-      <c r="C26" s="128"/>
+      <c r="B26" s="111"/>
+      <c r="C26" s="104"/>
       <c r="D26" s="48" t="s">
         <v>111</v>
       </c>
@@ -6060,8 +6168,8 @@
       <c r="F26" s="48" t="s">
         <v>298</v>
       </c>
-      <c r="G26" s="109"/>
-      <c r="H26" s="109"/>
+      <c r="G26" s="131"/>
+      <c r="H26" s="131"/>
       <c r="I26" s="48"/>
       <c r="J26" s="48" t="s">
         <v>156</v>
@@ -6075,8 +6183,8 @@
       <c r="O26" s="59"/>
     </row>
     <row r="27" spans="2:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="129"/>
-      <c r="C27" s="123" t="s">
+      <c r="B27" s="111"/>
+      <c r="C27" s="105" t="s">
         <v>119</v>
       </c>
       <c r="D27" s="47" t="s">
@@ -6088,10 +6196,10 @@
       <c r="F27" s="47" t="s">
         <v>299</v>
       </c>
-      <c r="G27" s="110" t="s">
+      <c r="G27" s="102" t="s">
         <v>255</v>
       </c>
-      <c r="H27" s="110" t="s">
+      <c r="H27" s="102" t="s">
         <v>256</v>
       </c>
       <c r="I27" s="47"/>
@@ -6105,8 +6213,8 @@
       <c r="O27" s="59"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B28" s="129"/>
-      <c r="C28" s="124"/>
+      <c r="B28" s="111"/>
+      <c r="C28" s="108"/>
       <c r="D28" s="47" t="s">
         <v>115</v>
       </c>
@@ -6116,8 +6224,8 @@
       <c r="F28" s="47" t="s">
         <v>300</v>
       </c>
-      <c r="G28" s="111"/>
-      <c r="H28" s="111"/>
+      <c r="G28" s="118"/>
+      <c r="H28" s="118"/>
       <c r="I28" s="47"/>
       <c r="J28" s="47"/>
       <c r="K28" s="47" t="s">
@@ -6129,8 +6237,8 @@
       <c r="O28" s="59"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B29" s="129"/>
-      <c r="C29" s="124"/>
+      <c r="B29" s="111"/>
+      <c r="C29" s="108"/>
       <c r="D29" s="47" t="s">
         <v>116</v>
       </c>
@@ -6140,8 +6248,8 @@
       <c r="F29" s="47" t="s">
         <v>301</v>
       </c>
-      <c r="G29" s="111"/>
-      <c r="H29" s="111"/>
+      <c r="G29" s="118"/>
+      <c r="H29" s="118"/>
       <c r="I29" s="47"/>
       <c r="J29" s="47" t="s">
         <v>159</v>
@@ -6153,8 +6261,8 @@
       <c r="O29" s="59"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B30" s="129"/>
-      <c r="C30" s="124"/>
+      <c r="B30" s="111"/>
+      <c r="C30" s="108"/>
       <c r="D30" s="47" t="s">
         <v>117</v>
       </c>
@@ -6164,8 +6272,8 @@
       <c r="F30" s="47" t="s">
         <v>302</v>
       </c>
-      <c r="G30" s="111"/>
-      <c r="H30" s="111"/>
+      <c r="G30" s="118"/>
+      <c r="H30" s="118"/>
       <c r="I30" s="47"/>
       <c r="J30" s="47" t="s">
         <v>160</v>
@@ -6177,9 +6285,9 @@
       <c r="O30" s="59"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B31" s="129"/>
-      <c r="C31" s="124"/>
-      <c r="D31" s="110" t="s">
+      <c r="B31" s="111"/>
+      <c r="C31" s="108"/>
+      <c r="D31" s="102" t="s">
         <v>118</v>
       </c>
       <c r="E31" s="60" t="s">
@@ -6188,8 +6296,8 @@
       <c r="F31" s="60" t="s">
         <v>303</v>
       </c>
-      <c r="G31" s="111"/>
-      <c r="H31" s="111"/>
+      <c r="G31" s="118"/>
+      <c r="H31" s="118"/>
       <c r="I31" s="60"/>
       <c r="J31" s="60"/>
       <c r="K31" s="60" t="s">
@@ -6201,17 +6309,17 @@
       <c r="O31" s="59"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B32" s="129"/>
-      <c r="C32" s="125"/>
-      <c r="D32" s="112"/>
+      <c r="B32" s="111"/>
+      <c r="C32" s="109"/>
+      <c r="D32" s="103"/>
       <c r="E32" s="60" t="s">
         <v>134</v>
       </c>
       <c r="F32" s="60" t="s">
         <v>304</v>
       </c>
-      <c r="G32" s="112"/>
-      <c r="H32" s="112"/>
+      <c r="G32" s="103"/>
+      <c r="H32" s="103"/>
       <c r="I32" s="60"/>
       <c r="J32" s="60" t="s">
         <v>131</v>
@@ -6225,25 +6333,25 @@
       <c r="O32" s="59"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B33" s="128" t="s">
+      <c r="B33" s="104" t="s">
         <v>151</v>
       </c>
-      <c r="C33" s="128" t="s">
+      <c r="C33" s="104" t="s">
         <v>150</v>
       </c>
-      <c r="D33" s="122" t="s">
+      <c r="D33" s="110" t="s">
         <v>137</v>
       </c>
-      <c r="E33" s="101" t="s">
+      <c r="E33" s="112" t="s">
         <v>141</v>
       </c>
       <c r="F33" s="50" t="s">
         <v>305</v>
       </c>
-      <c r="G33" s="119" t="s">
+      <c r="G33" s="124" t="s">
         <v>257</v>
       </c>
-      <c r="H33" s="122" t="s">
+      <c r="H33" s="110" t="s">
         <v>258</v>
       </c>
       <c r="I33" s="51"/>
@@ -6257,15 +6365,15 @@
       <c r="O33" s="59"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B34" s="129"/>
-      <c r="C34" s="129"/>
-      <c r="D34" s="122"/>
-      <c r="E34" s="103"/>
+      <c r="B34" s="111"/>
+      <c r="C34" s="111"/>
+      <c r="D34" s="110"/>
+      <c r="E34" s="113"/>
       <c r="F34" s="50" t="s">
         <v>306</v>
       </c>
-      <c r="G34" s="120"/>
-      <c r="H34" s="122"/>
+      <c r="G34" s="125"/>
+      <c r="H34" s="110"/>
       <c r="I34" s="66"/>
       <c r="J34" s="50" t="s">
         <v>152</v>
@@ -6277,8 +6385,8 @@
       <c r="O34" s="59"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B35" s="129"/>
-      <c r="C35" s="129"/>
+      <c r="B35" s="111"/>
+      <c r="C35" s="111"/>
       <c r="D35" s="50" t="s">
         <v>138</v>
       </c>
@@ -6288,8 +6396,8 @@
       <c r="F35" s="50" t="s">
         <v>307</v>
       </c>
-      <c r="G35" s="120"/>
-      <c r="H35" s="122"/>
+      <c r="G35" s="125"/>
+      <c r="H35" s="110"/>
       <c r="I35" s="66"/>
       <c r="J35" s="50"/>
       <c r="K35" s="50" t="s">
@@ -6301,8 +6409,8 @@
       <c r="O35" s="59"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B36" s="129"/>
-      <c r="C36" s="129"/>
+      <c r="B36" s="111"/>
+      <c r="C36" s="111"/>
       <c r="D36" s="50" t="s">
         <v>139</v>
       </c>
@@ -6312,8 +6420,8 @@
       <c r="F36" s="50" t="s">
         <v>308</v>
       </c>
-      <c r="G36" s="120"/>
-      <c r="H36" s="122"/>
+      <c r="G36" s="125"/>
+      <c r="H36" s="110"/>
       <c r="I36" s="66"/>
       <c r="J36" s="50" t="s">
         <v>161</v>
@@ -6327,19 +6435,19 @@
       <c r="O36" s="59"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B37" s="129"/>
-      <c r="C37" s="129"/>
+      <c r="B37" s="111"/>
+      <c r="C37" s="111"/>
       <c r="D37" s="50" t="s">
         <v>140</v>
       </c>
-      <c r="E37" s="101" t="s">
+      <c r="E37" s="112" t="s">
         <v>148</v>
       </c>
       <c r="F37" s="50" t="s">
         <v>309</v>
       </c>
-      <c r="G37" s="120"/>
-      <c r="H37" s="122"/>
+      <c r="G37" s="125"/>
+      <c r="H37" s="110"/>
       <c r="I37" s="66"/>
       <c r="J37" s="50"/>
       <c r="K37" s="50" t="s">
@@ -6351,15 +6459,15 @@
       <c r="O37" s="59"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B38" s="129"/>
-      <c r="C38" s="129"/>
+      <c r="B38" s="111"/>
+      <c r="C38" s="111"/>
       <c r="D38" s="50"/>
-      <c r="E38" s="103"/>
+      <c r="E38" s="113"/>
       <c r="F38" s="50" t="s">
         <v>310</v>
       </c>
-      <c r="G38" s="120"/>
-      <c r="H38" s="122"/>
+      <c r="G38" s="125"/>
+      <c r="H38" s="110"/>
       <c r="I38" s="66"/>
       <c r="J38" s="50" t="s">
         <v>152</v>
@@ -6371,8 +6479,8 @@
       <c r="O38" s="59"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B39" s="129"/>
-      <c r="C39" s="129"/>
+      <c r="B39" s="111"/>
+      <c r="C39" s="111"/>
       <c r="D39" s="50" t="s">
         <v>144</v>
       </c>
@@ -6382,8 +6490,8 @@
       <c r="F39" s="50" t="s">
         <v>311</v>
       </c>
-      <c r="G39" s="120"/>
-      <c r="H39" s="122"/>
+      <c r="G39" s="125"/>
+      <c r="H39" s="110"/>
       <c r="I39" s="66"/>
       <c r="J39" s="50" t="s">
         <v>161</v>
@@ -6395,19 +6503,19 @@
       <c r="O39" s="59"/>
     </row>
     <row r="40" spans="2:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="129"/>
-      <c r="C40" s="129"/>
-      <c r="D40" s="101" t="s">
+      <c r="B40" s="111"/>
+      <c r="C40" s="111"/>
+      <c r="D40" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="E40" s="101" t="s">
+      <c r="E40" s="112" t="s">
         <v>146</v>
       </c>
       <c r="F40" s="50" t="s">
         <v>312</v>
       </c>
-      <c r="G40" s="120"/>
-      <c r="H40" s="122"/>
+      <c r="G40" s="125"/>
+      <c r="H40" s="110"/>
       <c r="I40" s="66"/>
       <c r="J40" s="50" t="s">
         <v>152</v>
@@ -6421,15 +6529,15 @@
       <c r="O40" s="59"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B41" s="129"/>
-      <c r="C41" s="129"/>
-      <c r="D41" s="103"/>
-      <c r="E41" s="103"/>
+      <c r="B41" s="111"/>
+      <c r="C41" s="111"/>
+      <c r="D41" s="113"/>
+      <c r="E41" s="113"/>
       <c r="F41" s="71" t="s">
         <v>312</v>
       </c>
-      <c r="G41" s="121"/>
-      <c r="H41" s="122"/>
+      <c r="G41" s="126"/>
+      <c r="H41" s="110"/>
       <c r="I41" s="66"/>
       <c r="J41" s="50" t="s">
         <v>152</v>
@@ -6441,8 +6549,8 @@
       <c r="O41" s="59"/>
     </row>
     <row r="42" spans="2:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="129"/>
-      <c r="C42" s="128" t="s">
+      <c r="B42" s="111"/>
+      <c r="C42" s="104" t="s">
         <v>120</v>
       </c>
       <c r="D42" s="50" t="s">
@@ -6454,10 +6562,10 @@
       <c r="F42" s="50" t="s">
         <v>313</v>
       </c>
-      <c r="G42" s="101" t="s">
+      <c r="G42" s="112" t="s">
         <v>251</v>
       </c>
-      <c r="H42" s="101" t="s">
+      <c r="H42" s="112" t="s">
         <v>252</v>
       </c>
       <c r="I42" s="50"/>
@@ -6473,8 +6581,8 @@
       <c r="O42" s="59"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B43" s="129"/>
-      <c r="C43" s="128"/>
+      <c r="B43" s="111"/>
+      <c r="C43" s="104"/>
       <c r="D43" s="50" t="s">
         <v>74</v>
       </c>
@@ -6484,8 +6592,8 @@
       <c r="F43" s="50" t="s">
         <v>314</v>
       </c>
-      <c r="G43" s="102"/>
-      <c r="H43" s="102"/>
+      <c r="G43" s="127"/>
+      <c r="H43" s="127"/>
       <c r="I43" s="50"/>
       <c r="J43" s="50"/>
       <c r="K43" s="50" t="s">
@@ -6497,8 +6605,8 @@
       <c r="O43" s="59"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B44" s="129"/>
-      <c r="C44" s="128"/>
+      <c r="B44" s="111"/>
+      <c r="C44" s="104"/>
       <c r="D44" s="50" t="s">
         <v>122</v>
       </c>
@@ -6508,8 +6616,8 @@
       <c r="F44" s="50" t="s">
         <v>315</v>
       </c>
-      <c r="G44" s="103"/>
-      <c r="H44" s="103"/>
+      <c r="G44" s="113"/>
+      <c r="H44" s="113"/>
       <c r="I44" s="50"/>
       <c r="J44" s="50" t="s">
         <v>81</v>
@@ -6556,11 +6664,30 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C16:C22"/>
-    <mergeCell ref="C10:C15"/>
-    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="G42:G44"/>
+    <mergeCell ref="H42:H44"/>
+    <mergeCell ref="G16:G22"/>
+    <mergeCell ref="H16:H22"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="H23:H26"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="H27:H32"/>
+    <mergeCell ref="G3:G9"/>
+    <mergeCell ref="H3:H9"/>
+    <mergeCell ref="G10:G15"/>
+    <mergeCell ref="H10:H15"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="G33:G41"/>
+    <mergeCell ref="H33:H41"/>
     <mergeCell ref="D31:D32"/>
     <mergeCell ref="C27:C32"/>
     <mergeCell ref="C3:C9"/>
@@ -6577,30 +6704,11 @@
     <mergeCell ref="C23:C26"/>
     <mergeCell ref="C42:C44"/>
     <mergeCell ref="D10:D11"/>
-    <mergeCell ref="G3:G9"/>
-    <mergeCell ref="H3:H9"/>
-    <mergeCell ref="G10:G15"/>
-    <mergeCell ref="H10:H15"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="G33:G41"/>
-    <mergeCell ref="H33:H41"/>
-    <mergeCell ref="G42:G44"/>
-    <mergeCell ref="H42:H44"/>
-    <mergeCell ref="G16:G22"/>
-    <mergeCell ref="H16:H22"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="H23:H26"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="H27:H32"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C16:C22"/>
+    <mergeCell ref="C10:C15"/>
+    <mergeCell ref="D16:D17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6659,22 +6767,22 @@
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="142" t="s">
+      <c r="B3" s="133" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="141" t="s">
+      <c r="C3" s="132" t="s">
         <v>195</v>
       </c>
-      <c r="D3" s="141" t="s">
+      <c r="D3" s="132" t="s">
         <v>187</v>
       </c>
       <c r="E3" s="61" t="s">
         <v>272</v>
       </c>
-      <c r="F3" s="141" t="s">
+      <c r="F3" s="132" t="s">
         <v>202</v>
       </c>
-      <c r="G3" s="141" t="s">
+      <c r="G3" s="132" t="s">
         <v>203</v>
       </c>
       <c r="H3" s="61" t="s">
@@ -6685,14 +6793,14 @@
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="142"/>
-      <c r="C4" s="141"/>
-      <c r="D4" s="141"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="132"/>
+      <c r="D4" s="132"/>
       <c r="E4" s="73" t="s">
         <v>276</v>
       </c>
-      <c r="F4" s="141"/>
-      <c r="G4" s="141"/>
+      <c r="F4" s="132"/>
+      <c r="G4" s="132"/>
       <c r="H4" s="61" t="s">
         <v>206</v>
       </c>
@@ -6701,30 +6809,30 @@
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="142"/>
-      <c r="C5" s="141"/>
-      <c r="D5" s="141" t="s">
+      <c r="B5" s="133"/>
+      <c r="C5" s="132"/>
+      <c r="D5" s="132" t="s">
         <v>188</v>
       </c>
       <c r="E5" s="73" t="s">
         <v>317</v>
       </c>
-      <c r="F5" s="141"/>
-      <c r="G5" s="141"/>
+      <c r="F5" s="132"/>
+      <c r="G5" s="132"/>
       <c r="H5" s="61"/>
       <c r="I5" s="61" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="142"/>
-      <c r="C6" s="141"/>
-      <c r="D6" s="141"/>
+      <c r="B6" s="133"/>
+      <c r="C6" s="132"/>
+      <c r="D6" s="132"/>
       <c r="E6" s="61" t="s">
         <v>316</v>
       </c>
-      <c r="F6" s="141"/>
-      <c r="G6" s="141"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="132"/>
       <c r="H6" s="61" t="s">
         <v>208</v>
       </c>
@@ -6733,30 +6841,30 @@
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="142"/>
-      <c r="C7" s="141"/>
-      <c r="D7" s="141" t="s">
+      <c r="B7" s="133"/>
+      <c r="C7" s="132"/>
+      <c r="D7" s="132" t="s">
         <v>189</v>
       </c>
       <c r="E7" s="61" t="s">
         <v>318</v>
       </c>
-      <c r="F7" s="141"/>
-      <c r="G7" s="141"/>
+      <c r="F7" s="132"/>
+      <c r="G7" s="132"/>
       <c r="H7" s="61"/>
       <c r="I7" s="61" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="142"/>
-      <c r="C8" s="141"/>
-      <c r="D8" s="141"/>
+      <c r="B8" s="133"/>
+      <c r="C8" s="132"/>
+      <c r="D8" s="132"/>
       <c r="E8" s="61" t="s">
         <v>318</v>
       </c>
-      <c r="F8" s="141"/>
-      <c r="G8" s="141"/>
+      <c r="F8" s="132"/>
+      <c r="G8" s="132"/>
       <c r="H8" s="61" t="s">
         <v>209</v>
       </c>
@@ -6765,30 +6873,30 @@
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="142"/>
-      <c r="C9" s="141"/>
-      <c r="D9" s="141" t="s">
+      <c r="B9" s="133"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="132" t="s">
         <v>190</v>
       </c>
       <c r="E9" s="61" t="s">
         <v>319</v>
       </c>
-      <c r="F9" s="141"/>
-      <c r="G9" s="141"/>
+      <c r="F9" s="132"/>
+      <c r="G9" s="132"/>
       <c r="H9" s="61"/>
       <c r="I9" s="61" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="142"/>
-      <c r="C10" s="141"/>
-      <c r="D10" s="141"/>
+      <c r="B10" s="133"/>
+      <c r="C10" s="132"/>
+      <c r="D10" s="132"/>
       <c r="E10" s="61" t="s">
         <v>320</v>
       </c>
-      <c r="F10" s="141"/>
-      <c r="G10" s="141"/>
+      <c r="F10" s="132"/>
+      <c r="G10" s="132"/>
       <c r="H10" s="61" t="s">
         <v>210</v>
       </c>
@@ -6797,7 +6905,7 @@
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="142"/>
+      <c r="B11" s="133"/>
       <c r="C11" s="61" t="s">
         <v>194</v>
       </c>
@@ -6821,7 +6929,7 @@
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="142"/>
+      <c r="B12" s="133"/>
       <c r="C12" s="61" t="s">
         <v>193</v>
       </c>
@@ -6881,22 +6989,22 @@
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="136" t="s">
+      <c r="B15" s="138" t="s">
         <v>234</v>
       </c>
-      <c r="C15" s="141" t="s">
+      <c r="C15" s="132" t="s">
         <v>195</v>
       </c>
-      <c r="D15" s="141" t="s">
+      <c r="D15" s="132" t="s">
         <v>188</v>
       </c>
       <c r="E15" s="61" t="s">
         <v>321</v>
       </c>
-      <c r="F15" s="137" t="s">
+      <c r="F15" s="139" t="s">
         <v>235</v>
       </c>
-      <c r="G15" s="137" t="s">
+      <c r="G15" s="139" t="s">
         <v>236</v>
       </c>
       <c r="H15" s="61"/>
@@ -6905,14 +7013,14 @@
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="136"/>
-      <c r="C16" s="141"/>
-      <c r="D16" s="141"/>
+      <c r="B16" s="138"/>
+      <c r="C16" s="132"/>
+      <c r="D16" s="132"/>
       <c r="E16" s="61" t="s">
         <v>322</v>
       </c>
-      <c r="F16" s="138"/>
-      <c r="G16" s="138"/>
+      <c r="F16" s="140"/>
+      <c r="G16" s="140"/>
       <c r="H16" s="61" t="s">
         <v>237</v>
       </c>
@@ -6921,32 +7029,32 @@
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="136"/>
-      <c r="C17" s="141"/>
+      <c r="B17" s="138"/>
+      <c r="C17" s="132"/>
       <c r="D17" s="61" t="s">
         <v>225</v>
       </c>
       <c r="E17" s="61" t="s">
         <v>323</v>
       </c>
-      <c r="F17" s="138"/>
-      <c r="G17" s="138"/>
+      <c r="F17" s="140"/>
+      <c r="G17" s="140"/>
       <c r="H17" s="61"/>
       <c r="I17" s="61" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="136"/>
-      <c r="C18" s="141"/>
+      <c r="B18" s="138"/>
+      <c r="C18" s="132"/>
       <c r="D18" s="61" t="s">
         <v>242</v>
       </c>
       <c r="E18" s="61" t="s">
         <v>324</v>
       </c>
-      <c r="F18" s="138"/>
-      <c r="G18" s="138"/>
+      <c r="F18" s="140"/>
+      <c r="G18" s="140"/>
       <c r="H18" s="61" t="s">
         <v>243</v>
       </c>
@@ -6955,16 +7063,16 @@
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="136"/>
-      <c r="C19" s="141"/>
+      <c r="B19" s="138"/>
+      <c r="C19" s="132"/>
       <c r="D19" s="61" t="s">
         <v>226</v>
       </c>
       <c r="E19" s="61" t="s">
         <v>325</v>
       </c>
-      <c r="F19" s="139"/>
-      <c r="G19" s="139"/>
+      <c r="F19" s="141"/>
+      <c r="G19" s="141"/>
       <c r="H19" s="61" t="s">
         <v>238</v>
       </c>
@@ -6973,66 +7081,66 @@
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="136"/>
-      <c r="C20" s="132" t="s">
+      <c r="B20" s="138"/>
+      <c r="C20" s="134" t="s">
         <v>233</v>
       </c>
-      <c r="D20" s="132" t="s">
+      <c r="D20" s="134" t="s">
         <v>227</v>
       </c>
       <c r="E20" s="61" t="s">
         <v>328</v>
       </c>
-      <c r="F20" s="133" t="s">
+      <c r="F20" s="135" t="s">
         <v>245</v>
       </c>
-      <c r="G20" s="133" t="s">
+      <c r="G20" s="135" t="s">
         <v>246</v>
       </c>
       <c r="H20" s="61"/>
       <c r="I20" s="61"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="136"/>
-      <c r="C21" s="132"/>
-      <c r="D21" s="132"/>
+      <c r="B21" s="138"/>
+      <c r="C21" s="134"/>
+      <c r="D21" s="134"/>
       <c r="E21" s="61" t="s">
         <v>329</v>
       </c>
-      <c r="F21" s="134"/>
-      <c r="G21" s="134"/>
+      <c r="F21" s="136"/>
+      <c r="G21" s="136"/>
       <c r="H21" s="61"/>
       <c r="I21" s="61"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="136"/>
-      <c r="C22" s="132"/>
-      <c r="D22" s="132" t="s">
+      <c r="B22" s="138"/>
+      <c r="C22" s="134"/>
+      <c r="D22" s="134" t="s">
         <v>228</v>
       </c>
       <c r="E22" s="61" t="s">
         <v>330</v>
       </c>
-      <c r="F22" s="134"/>
-      <c r="G22" s="134"/>
+      <c r="F22" s="136"/>
+      <c r="G22" s="136"/>
       <c r="H22" s="61"/>
       <c r="I22" s="61"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="136"/>
-      <c r="C23" s="132"/>
-      <c r="D23" s="132"/>
+      <c r="B23" s="138"/>
+      <c r="C23" s="134"/>
+      <c r="D23" s="134"/>
       <c r="E23" s="73" t="s">
         <v>331</v>
       </c>
-      <c r="F23" s="135"/>
-      <c r="G23" s="135"/>
+      <c r="F23" s="137"/>
+      <c r="G23" s="137"/>
       <c r="H23" s="61"/>
       <c r="I23" s="61"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="136"/>
-      <c r="C24" s="132" t="s">
+      <c r="B24" s="138"/>
+      <c r="C24" s="134" t="s">
         <v>232</v>
       </c>
       <c r="D24" s="61" t="s">
@@ -7047,9 +7155,9 @@
       <c r="I24" s="61"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="136"/>
-      <c r="C25" s="132"/>
-      <c r="D25" s="132" t="s">
+      <c r="B25" s="138"/>
+      <c r="C25" s="134"/>
+      <c r="D25" s="134" t="s">
         <v>231</v>
       </c>
       <c r="E25" s="61" t="s">
@@ -7061,9 +7169,9 @@
       <c r="I25" s="61"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="136"/>
-      <c r="C26" s="132"/>
-      <c r="D26" s="132"/>
+      <c r="B26" s="138"/>
+      <c r="C26" s="134"/>
+      <c r="D26" s="134"/>
       <c r="E26" s="73" t="s">
         <v>334</v>
       </c>
@@ -7073,11 +7181,11 @@
       <c r="I26" s="61"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B27" s="136"/>
-      <c r="C27" s="132" t="s">
+      <c r="B27" s="138"/>
+      <c r="C27" s="134" t="s">
         <v>194</v>
       </c>
-      <c r="D27" s="132" t="s">
+      <c r="D27" s="134" t="s">
         <v>230</v>
       </c>
       <c r="E27" s="61" t="s">
@@ -7089,9 +7197,9 @@
       <c r="I27" s="61"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B28" s="136"/>
-      <c r="C28" s="132"/>
-      <c r="D28" s="132"/>
+      <c r="B28" s="138"/>
+      <c r="C28" s="134"/>
+      <c r="D28" s="134"/>
       <c r="E28" s="61" t="s">
         <v>336</v>
       </c>
@@ -7128,116 +7236,116 @@
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="140" t="s">
+      <c r="B31" s="142" t="s">
         <v>259</v>
       </c>
-      <c r="C31" s="141" t="s">
+      <c r="C31" s="132" t="s">
         <v>195</v>
       </c>
-      <c r="D31" s="141" t="s">
+      <c r="D31" s="132" t="s">
         <v>188</v>
       </c>
       <c r="E31" s="61" t="s">
         <v>337</v>
       </c>
-      <c r="F31" s="137" t="s">
+      <c r="F31" s="139" t="s">
         <v>202</v>
       </c>
-      <c r="G31" s="137" t="s">
+      <c r="G31" s="139" t="s">
         <v>203</v>
       </c>
       <c r="H31" s="61"/>
       <c r="I31" s="61"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B32" s="140"/>
-      <c r="C32" s="141"/>
-      <c r="D32" s="141"/>
+      <c r="B32" s="142"/>
+      <c r="C32" s="132"/>
+      <c r="D32" s="132"/>
       <c r="E32" s="61" t="s">
         <v>338</v>
       </c>
-      <c r="F32" s="138"/>
-      <c r="G32" s="138"/>
+      <c r="F32" s="140"/>
+      <c r="G32" s="140"/>
       <c r="H32" s="61"/>
       <c r="I32" s="61"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="140"/>
-      <c r="C33" s="141"/>
+      <c r="B33" s="142"/>
+      <c r="C33" s="132"/>
       <c r="D33" s="61" t="s">
         <v>225</v>
       </c>
       <c r="E33" s="61" t="s">
         <v>339</v>
       </c>
-      <c r="F33" s="138"/>
-      <c r="G33" s="138"/>
+      <c r="F33" s="140"/>
+      <c r="G33" s="140"/>
       <c r="H33" s="61"/>
       <c r="I33" s="61"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="140"/>
-      <c r="C34" s="141"/>
+      <c r="B34" s="142"/>
+      <c r="C34" s="132"/>
       <c r="D34" s="61"/>
       <c r="E34" s="61"/>
-      <c r="F34" s="138"/>
-      <c r="G34" s="138"/>
+      <c r="F34" s="140"/>
+      <c r="G34" s="140"/>
       <c r="H34" s="61"/>
       <c r="I34" s="61"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B35" s="140"/>
-      <c r="C35" s="141"/>
+      <c r="B35" s="142"/>
+      <c r="C35" s="132"/>
       <c r="D35" s="61"/>
       <c r="E35" s="61"/>
-      <c r="F35" s="139"/>
-      <c r="G35" s="139"/>
+      <c r="F35" s="141"/>
+      <c r="G35" s="141"/>
       <c r="H35" s="61"/>
       <c r="I35" s="61"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B36" s="140"/>
-      <c r="C36" s="132"/>
-      <c r="D36" s="132"/>
+      <c r="B36" s="142"/>
+      <c r="C36" s="134"/>
+      <c r="D36" s="134"/>
       <c r="E36" s="61"/>
-      <c r="F36" s="133"/>
-      <c r="G36" s="133"/>
+      <c r="F36" s="135"/>
+      <c r="G36" s="135"/>
       <c r="H36" s="61"/>
       <c r="I36" s="61"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B37" s="140"/>
-      <c r="C37" s="132"/>
-      <c r="D37" s="132"/>
+      <c r="B37" s="142"/>
+      <c r="C37" s="134"/>
+      <c r="D37" s="134"/>
       <c r="E37" s="61"/>
-      <c r="F37" s="134"/>
-      <c r="G37" s="134"/>
+      <c r="F37" s="136"/>
+      <c r="G37" s="136"/>
       <c r="H37" s="61"/>
       <c r="I37" s="61"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B38" s="140"/>
-      <c r="C38" s="132"/>
-      <c r="D38" s="132"/>
+      <c r="B38" s="142"/>
+      <c r="C38" s="134"/>
+      <c r="D38" s="134"/>
       <c r="E38" s="61"/>
-      <c r="F38" s="134"/>
-      <c r="G38" s="134"/>
+      <c r="F38" s="136"/>
+      <c r="G38" s="136"/>
       <c r="H38" s="61"/>
       <c r="I38" s="61"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B39" s="140"/>
-      <c r="C39" s="132"/>
-      <c r="D39" s="132"/>
+      <c r="B39" s="142"/>
+      <c r="C39" s="134"/>
+      <c r="D39" s="134"/>
       <c r="E39" s="61"/>
-      <c r="F39" s="135"/>
-      <c r="G39" s="135"/>
+      <c r="F39" s="137"/>
+      <c r="G39" s="137"/>
       <c r="H39" s="61"/>
       <c r="I39" s="61"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B40" s="140"/>
-      <c r="C40" s="132"/>
+      <c r="B40" s="142"/>
+      <c r="C40" s="134"/>
       <c r="D40" s="61"/>
       <c r="E40" s="61"/>
       <c r="F40" s="61"/>
@@ -7246,9 +7354,9 @@
       <c r="I40" s="61"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="140"/>
-      <c r="C41" s="132"/>
-      <c r="D41" s="132"/>
+      <c r="B41" s="142"/>
+      <c r="C41" s="134"/>
+      <c r="D41" s="134"/>
       <c r="E41" s="61"/>
       <c r="F41" s="61"/>
       <c r="G41" s="61"/>
@@ -7256,9 +7364,9 @@
       <c r="I41" s="61"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="140"/>
-      <c r="C42" s="132"/>
-      <c r="D42" s="132"/>
+      <c r="B42" s="142"/>
+      <c r="C42" s="134"/>
+      <c r="D42" s="134"/>
       <c r="E42" s="61"/>
       <c r="F42" s="61"/>
       <c r="G42" s="61"/>
@@ -7266,9 +7374,9 @@
       <c r="I42" s="61"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B43" s="140"/>
-      <c r="C43" s="132"/>
-      <c r="D43" s="132"/>
+      <c r="B43" s="142"/>
+      <c r="C43" s="134"/>
+      <c r="D43" s="134"/>
       <c r="E43" s="61"/>
       <c r="F43" s="61"/>
       <c r="G43" s="61"/>
@@ -7276,9 +7384,9 @@
       <c r="I43" s="61"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B44" s="140"/>
-      <c r="C44" s="132"/>
-      <c r="D44" s="132"/>
+      <c r="B44" s="142"/>
+      <c r="C44" s="134"/>
+      <c r="D44" s="134"/>
       <c r="E44" s="61"/>
       <c r="F44" s="61"/>
       <c r="G44" s="61"/>
@@ -7287,21 +7395,11 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="B3:B12"/>
-    <mergeCell ref="F3:F10"/>
-    <mergeCell ref="G3:G10"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="F36:F39"/>
     <mergeCell ref="G36:G39"/>
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="C40:C42"/>
@@ -7318,11 +7416,21 @@
     <mergeCell ref="G31:G35"/>
     <mergeCell ref="C15:C19"/>
     <mergeCell ref="D20:D21"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="F36:F39"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="C20:C23"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="B3:B12"/>
+    <mergeCell ref="F3:F10"/>
+    <mergeCell ref="G3:G10"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D9:D10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7334,8 +7442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -7360,31 +7468,39 @@
     </row>
     <row r="3" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="76" t="s">
+        <v>345</v>
+      </c>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75" t="s">
         <v>344</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
     </row>
     <row r="4" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="77" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
+      <c r="D4" s="76" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="5" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="76" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C5" s="76"/>
-      <c r="D5" s="78"/>
+      <c r="D5" s="78" t="s">
+        <v>348</v>
+      </c>
     </row>
     <row r="6" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="79" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
+      <c r="D6" s="78" t="s">
+        <v>350</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Auto push 2023-05-09 18:03:18.08
</commit_message>
<xml_diff>
--- a/note/10_2ndTeamProject/일정관리.xlsx
+++ b/note/10_2ndTeamProject/일정관리.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="8595" windowHeight="11730" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Gantt Chart" sheetId="4" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="355">
   <si>
     <t>이용자 권한과 기능</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1422,15 +1422,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DB user/pw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>프로젝트명(아이템)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스터디모집</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1460,10 +1452,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>제주도 홍보</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">강성빈, 김성연, 김훈, </t>
     </r>
@@ -1479,10 +1467,6 @@
       </rPr>
       <t>안중권</t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>애견 용품 쇼핑몰</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1515,10 +1499,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>놀이동산</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1544,12 +1524,44 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>회의록</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>제주어때</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BOWOW(애견몰)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>참조사이트url, ppt바탕색(작업분할도), 업무분장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>업무분장</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>HelloWorld(놀이동산)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>발표순서</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PRONECT(스터디모집)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1690,6 +1702,15 @@
       <b/>
       <sz val="25"/>
       <color rgb="FF0000FF"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -2177,32 +2198,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -2232,13 +2227,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="143">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2470,30 +2487,63 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2512,160 +2562,133 @@
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3034,61 +3057,61 @@
     <row r="1" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="84" t="s">
         <v>340</v>
       </c>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-      <c r="H2" s="95"/>
-      <c r="I2" s="95"/>
-      <c r="J2" s="95"/>
-      <c r="K2" s="95"/>
-      <c r="L2" s="95"/>
-      <c r="M2" s="95"/>
-      <c r="N2" s="95"/>
-      <c r="O2" s="95"/>
-      <c r="P2" s="95"/>
-      <c r="Q2" s="95"/>
-      <c r="R2" s="95"/>
-      <c r="S2" s="95"/>
-      <c r="T2" s="95"/>
-      <c r="U2" s="95"/>
-      <c r="V2" s="95"/>
-      <c r="W2" s="95"/>
-      <c r="X2" s="95"/>
-      <c r="Y2" s="95"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85"/>
+      <c r="O2" s="85"/>
+      <c r="P2" s="85"/>
+      <c r="Q2" s="85"/>
+      <c r="R2" s="85"/>
+      <c r="S2" s="85"/>
+      <c r="T2" s="85"/>
+      <c r="U2" s="85"/>
+      <c r="V2" s="85"/>
+      <c r="W2" s="85"/>
+      <c r="X2" s="85"/>
+      <c r="Y2" s="85"/>
       <c r="Z2" s="5"/>
       <c r="AA2" s="5"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
-      <c r="B3" s="95"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-      <c r="H3" s="95"/>
-      <c r="I3" s="95"/>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
-      <c r="N3" s="95"/>
-      <c r="O3" s="95"/>
-      <c r="P3" s="95"/>
-      <c r="Q3" s="95"/>
-      <c r="R3" s="95"/>
-      <c r="S3" s="95"/>
-      <c r="T3" s="95"/>
-      <c r="U3" s="95"/>
-      <c r="V3" s="95"/>
-      <c r="W3" s="95"/>
-      <c r="X3" s="95"/>
-      <c r="Y3" s="95"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="85"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="85"/>
+      <c r="N3" s="85"/>
+      <c r="O3" s="85"/>
+      <c r="P3" s="85"/>
+      <c r="Q3" s="85"/>
+      <c r="R3" s="85"/>
+      <c r="S3" s="85"/>
+      <c r="T3" s="85"/>
+      <c r="U3" s="85"/>
+      <c r="V3" s="85"/>
+      <c r="W3" s="85"/>
+      <c r="X3" s="85"/>
+      <c r="Y3" s="85"/>
       <c r="Z3" s="5"/>
       <c r="AA3" s="5"/>
     </row>
@@ -3153,44 +3176,44 @@
     <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="18"/>
       <c r="B6" s="22"/>
-      <c r="C6" s="96" t="s">
+      <c r="C6" s="86" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="23"/>
-      <c r="E6" s="83" t="s">
+      <c r="E6" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="83"/>
-      <c r="J6" s="83"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="82" t="s">
+      <c r="F6" s="88"/>
+      <c r="G6" s="88"/>
+      <c r="H6" s="88"/>
+      <c r="I6" s="88"/>
+      <c r="J6" s="88"/>
+      <c r="K6" s="89"/>
+      <c r="L6" s="95" t="s">
         <v>45</v>
       </c>
-      <c r="M6" s="83"/>
-      <c r="N6" s="83"/>
-      <c r="O6" s="83"/>
-      <c r="P6" s="83"/>
-      <c r="Q6" s="83"/>
-      <c r="R6" s="84"/>
-      <c r="S6" s="82" t="s">
+      <c r="M6" s="88"/>
+      <c r="N6" s="88"/>
+      <c r="O6" s="88"/>
+      <c r="P6" s="88"/>
+      <c r="Q6" s="88"/>
+      <c r="R6" s="89"/>
+      <c r="S6" s="95" t="s">
         <v>185</v>
       </c>
-      <c r="T6" s="83"/>
-      <c r="U6" s="83"/>
-      <c r="V6" s="83"/>
-      <c r="W6" s="83"/>
-      <c r="X6" s="83"/>
-      <c r="Y6" s="83"/>
+      <c r="T6" s="88"/>
+      <c r="U6" s="88"/>
+      <c r="V6" s="88"/>
+      <c r="W6" s="88"/>
+      <c r="X6" s="88"/>
+      <c r="Y6" s="88"/>
       <c r="Z6" s="24"/>
       <c r="AA6" s="5"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="18"/>
       <c r="B7" s="15"/>
-      <c r="C7" s="97"/>
+      <c r="C7" s="87"/>
       <c r="D7" s="25"/>
       <c r="E7" s="15">
         <v>13</v>
@@ -3346,7 +3369,7 @@
     <row r="11" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="6"/>
-      <c r="C11" s="98" t="s">
+      <c r="C11" s="90" t="s">
         <v>43</v>
       </c>
       <c r="D11" s="42"/>
@@ -3377,7 +3400,7 @@
     <row r="12" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="6"/>
-      <c r="C12" s="98"/>
+      <c r="C12" s="90"/>
       <c r="D12" s="41"/>
       <c r="E12" s="8"/>
       <c r="F12" s="6"/>
@@ -3435,7 +3458,7 @@
     <row r="14" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="6"/>
-      <c r="C14" s="99" t="s">
+      <c r="C14" s="92" t="s">
         <v>44</v>
       </c>
       <c r="D14" s="11"/>
@@ -3466,7 +3489,7 @@
     <row r="15" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="6"/>
-      <c r="C15" s="99"/>
+      <c r="C15" s="92"/>
       <c r="D15" s="11"/>
       <c r="E15" s="8"/>
       <c r="F15" s="6"/>
@@ -3524,7 +3547,7 @@
     <row r="17" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="6"/>
-      <c r="C17" s="98" t="s">
+      <c r="C17" s="90" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="10"/>
@@ -3555,7 +3578,7 @@
     <row r="18" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="18"/>
       <c r="B18" s="6"/>
-      <c r="C18" s="98"/>
+      <c r="C18" s="90"/>
       <c r="D18" s="10"/>
       <c r="E18" s="6"/>
       <c r="F18" s="8"/>
@@ -4209,7 +4232,7 @@
     <row r="40" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="18"/>
       <c r="B40" s="6"/>
-      <c r="C40" s="92" t="s">
+      <c r="C40" s="82" t="s">
         <v>30</v>
       </c>
       <c r="D40" s="12"/>
@@ -4240,7 +4263,7 @@
     <row r="41" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18"/>
       <c r="B41" s="6"/>
-      <c r="C41" s="92"/>
+      <c r="C41" s="82"/>
       <c r="D41" s="12"/>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
@@ -4298,7 +4321,7 @@
     <row r="43" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18"/>
       <c r="B43" s="6"/>
-      <c r="C43" s="92" t="s">
+      <c r="C43" s="82" t="s">
         <v>29</v>
       </c>
       <c r="D43" s="12"/>
@@ -4329,7 +4352,7 @@
     <row r="44" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="18"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="92"/>
+      <c r="C44" s="82"/>
       <c r="D44" s="12"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
@@ -4387,7 +4410,7 @@
     <row r="46" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="18"/>
       <c r="B46" s="6"/>
-      <c r="C46" s="92" t="s">
+      <c r="C46" s="82" t="s">
         <v>2</v>
       </c>
       <c r="D46" s="12"/>
@@ -4418,7 +4441,7 @@
     <row r="47" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="18"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="92"/>
+      <c r="C47" s="82"/>
       <c r="D47" s="12"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
@@ -4476,7 +4499,7 @@
     <row r="49" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="18"/>
       <c r="B49" s="6"/>
-      <c r="C49" s="92" t="s">
+      <c r="C49" s="82" t="s">
         <v>37</v>
       </c>
       <c r="D49" s="12"/>
@@ -4507,7 +4530,7 @@
     <row r="50" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="18"/>
       <c r="B50" s="6"/>
-      <c r="C50" s="92"/>
+      <c r="C50" s="82"/>
       <c r="D50" s="12"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
@@ -4596,7 +4619,7 @@
     <row r="53" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="18"/>
       <c r="B53" s="6"/>
-      <c r="C53" s="81" t="s">
+      <c r="C53" s="93" t="s">
         <v>32</v>
       </c>
       <c r="D53" s="10"/>
@@ -4627,7 +4650,7 @@
     <row r="54" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="18"/>
       <c r="B54" s="6"/>
-      <c r="C54" s="81"/>
+      <c r="C54" s="93"/>
       <c r="D54" s="10"/>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
@@ -4685,7 +4708,7 @@
     <row r="56" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="18"/>
       <c r="B56" s="6"/>
-      <c r="C56" s="81" t="s">
+      <c r="C56" s="93" t="s">
         <v>33</v>
       </c>
       <c r="D56" s="10"/>
@@ -4716,7 +4739,7 @@
     <row r="57" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="18"/>
       <c r="B57" s="6"/>
-      <c r="C57" s="81"/>
+      <c r="C57" s="93"/>
       <c r="D57" s="10"/>
       <c r="E57" s="6"/>
       <c r="F57" s="6"/>
@@ -4774,7 +4797,7 @@
     <row r="59" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="18"/>
       <c r="B59" s="6"/>
-      <c r="C59" s="81" t="s">
+      <c r="C59" s="93" t="s">
         <v>34</v>
       </c>
       <c r="D59" s="10"/>
@@ -4805,7 +4828,7 @@
     <row r="60" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="18"/>
       <c r="B60" s="6"/>
-      <c r="C60" s="81"/>
+      <c r="C60" s="93"/>
       <c r="D60" s="10"/>
       <c r="E60" s="6"/>
       <c r="F60" s="6"/>
@@ -4863,7 +4886,7 @@
     <row r="62" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="18"/>
       <c r="B62" s="6"/>
-      <c r="C62" s="81" t="s">
+      <c r="C62" s="93" t="s">
         <v>35</v>
       </c>
       <c r="D62" s="10"/>
@@ -4894,7 +4917,7 @@
     <row r="63" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="18"/>
       <c r="B63" s="6"/>
-      <c r="C63" s="81"/>
+      <c r="C63" s="93"/>
       <c r="D63" s="10"/>
       <c r="E63" s="6"/>
       <c r="F63" s="6"/>
@@ -4952,7 +4975,7 @@
     <row r="65" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="18"/>
       <c r="B65" s="6"/>
-      <c r="C65" s="81" t="s">
+      <c r="C65" s="93" t="s">
         <v>36</v>
       </c>
       <c r="D65" s="12"/>
@@ -4983,7 +5006,7 @@
     <row r="66" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="18"/>
       <c r="B66" s="6"/>
-      <c r="C66" s="81"/>
+      <c r="C66" s="93"/>
       <c r="D66" s="12"/>
       <c r="E66" s="6"/>
       <c r="F66" s="6"/>
@@ -5041,7 +5064,7 @@
     <row r="68" spans="1:27" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="18"/>
       <c r="B68" s="6"/>
-      <c r="C68" s="93" t="s">
+      <c r="C68" s="83" t="s">
         <v>167</v>
       </c>
       <c r="D68" s="7"/>
@@ -5072,7 +5095,7 @@
     <row r="69" spans="1:27" ht="6.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="18"/>
       <c r="B69" s="6"/>
-      <c r="C69" s="93"/>
+      <c r="C69" s="83"/>
       <c r="D69" s="7"/>
       <c r="E69" s="6"/>
       <c r="F69" s="6"/>
@@ -5161,40 +5184,40 @@
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
-      <c r="E72" s="80" t="s">
+      <c r="E72" s="94" t="s">
         <v>186</v>
       </c>
-      <c r="F72" s="80"/>
+      <c r="F72" s="94"/>
       <c r="G72" s="58"/>
-      <c r="H72" s="90" t="s">
+      <c r="H72" s="101" t="s">
         <v>184</v>
       </c>
-      <c r="I72" s="90"/>
+      <c r="I72" s="101"/>
       <c r="J72" s="57"/>
-      <c r="K72" s="89" t="s">
+      <c r="K72" s="100" t="s">
         <v>183</v>
       </c>
-      <c r="L72" s="89"/>
+      <c r="L72" s="100"/>
       <c r="M72" s="57"/>
-      <c r="N72" s="88" t="s">
+      <c r="N72" s="99" t="s">
         <v>182</v>
       </c>
-      <c r="O72" s="88"/>
+      <c r="O72" s="99"/>
       <c r="P72" s="57"/>
-      <c r="Q72" s="87" t="s">
+      <c r="Q72" s="98" t="s">
         <v>181</v>
       </c>
-      <c r="R72" s="87"/>
+      <c r="R72" s="98"/>
       <c r="S72" s="57"/>
-      <c r="T72" s="86" t="s">
+      <c r="T72" s="97" t="s">
         <v>180</v>
       </c>
-      <c r="U72" s="86"/>
+      <c r="U72" s="97"/>
       <c r="V72" s="57"/>
-      <c r="W72" s="85" t="s">
+      <c r="W72" s="96" t="s">
         <v>179</v>
       </c>
-      <c r="X72" s="85"/>
+      <c r="X72" s="96"/>
       <c r="Y72" s="5"/>
       <c r="Z72" s="5"/>
       <c r="AA72" s="5"/>
@@ -5229,21 +5252,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="B2:Y3"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="E6:K6"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="C46:C47"/>
     <mergeCell ref="E72:F72"/>
     <mergeCell ref="C59:C60"/>
     <mergeCell ref="C62:C63"/>
@@ -5260,6 +5268,21 @@
     <mergeCell ref="C53:C54"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="C43:C44"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="B2:Y3"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E6:K6"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C46:C47"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5288,7 +5311,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="100" t="s">
+      <c r="A3" s="102" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -5299,7 +5322,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="100"/>
+      <c r="A4" s="102"/>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -5311,7 +5334,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="100"/>
+      <c r="A5" s="102"/>
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -5326,7 +5349,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="100"/>
+      <c r="A6" s="102"/>
       <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
@@ -5569,25 +5592,25 @@
       <c r="N2" s="59"/>
     </row>
     <row r="3" spans="2:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="105" t="s">
+      <c r="B3" s="125" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="105" t="s">
+      <c r="C3" s="125" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="114" t="s">
+      <c r="D3" s="115" t="s">
         <v>53</v>
       </c>
-      <c r="E3" s="114" t="s">
+      <c r="E3" s="115" t="s">
         <v>59</v>
       </c>
       <c r="F3" s="65" t="s">
         <v>273</v>
       </c>
-      <c r="G3" s="114" t="s">
+      <c r="G3" s="115" t="s">
         <v>249</v>
       </c>
-      <c r="H3" s="114" t="s">
+      <c r="H3" s="115" t="s">
         <v>250</v>
       </c>
       <c r="I3" s="65" t="s">
@@ -5605,10 +5628,10 @@
       <c r="O3" s="59"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B4" s="106"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
+      <c r="B4" s="128"/>
+      <c r="C4" s="128"/>
+      <c r="D4" s="117"/>
+      <c r="E4" s="117"/>
       <c r="F4" s="65" t="s">
         <v>275</v>
       </c>
@@ -5631,12 +5654,12 @@
       <c r="O4" s="59"/>
     </row>
     <row r="5" spans="2:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="106"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="114" t="s">
+      <c r="B5" s="128"/>
+      <c r="C5" s="128"/>
+      <c r="D5" s="115" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="114" t="s">
+      <c r="E5" s="115" t="s">
         <v>56</v>
       </c>
       <c r="F5" s="65" t="s">
@@ -5657,10 +5680,10 @@
       <c r="O5" s="59"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="106"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="115"/>
-      <c r="E6" s="115"/>
+      <c r="B6" s="128"/>
+      <c r="C6" s="128"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="117"/>
       <c r="F6" s="65" t="s">
         <v>276</v>
       </c>
@@ -5683,12 +5706,12 @@
       <c r="O6" s="59"/>
     </row>
     <row r="7" spans="2:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="106"/>
-      <c r="C7" s="106"/>
-      <c r="D7" s="114" t="s">
+      <c r="B7" s="128"/>
+      <c r="C7" s="128"/>
+      <c r="D7" s="115" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="121" t="s">
+      <c r="E7" s="118" t="s">
         <v>94</v>
       </c>
       <c r="F7" s="65" t="s">
@@ -5711,10 +5734,10 @@
       <c r="O7" s="59"/>
     </row>
     <row r="8" spans="2:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="106"/>
-      <c r="C8" s="106"/>
+      <c r="B8" s="128"/>
+      <c r="C8" s="128"/>
       <c r="D8" s="116"/>
-      <c r="E8" s="122"/>
+      <c r="E8" s="119"/>
       <c r="F8" s="65" t="s">
         <v>277</v>
       </c>
@@ -5735,15 +5758,15 @@
       <c r="O8" s="59"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B9" s="107"/>
-      <c r="C9" s="107"/>
-      <c r="D9" s="115"/>
-      <c r="E9" s="123"/>
+      <c r="B9" s="129"/>
+      <c r="C9" s="129"/>
+      <c r="D9" s="117"/>
+      <c r="E9" s="120"/>
       <c r="F9" s="65" t="s">
         <v>279</v>
       </c>
-      <c r="G9" s="115"/>
-      <c r="H9" s="115"/>
+      <c r="G9" s="117"/>
+      <c r="H9" s="117"/>
       <c r="I9" s="65"/>
       <c r="J9" s="65"/>
       <c r="K9" s="65" t="s">
@@ -5755,25 +5778,25 @@
       <c r="O9" s="59"/>
     </row>
     <row r="10" spans="2:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="108" t="s">
+      <c r="B10" s="126" t="s">
         <v>166</v>
       </c>
-      <c r="C10" s="105" t="s">
+      <c r="C10" s="125" t="s">
         <v>165</v>
       </c>
-      <c r="D10" s="117" t="s">
+      <c r="D10" s="132" t="s">
         <v>69</v>
       </c>
-      <c r="E10" s="102" t="s">
+      <c r="E10" s="112" t="s">
         <v>70</v>
       </c>
       <c r="F10" s="47" t="s">
         <v>282</v>
       </c>
-      <c r="G10" s="102" t="s">
+      <c r="G10" s="112" t="s">
         <v>251</v>
       </c>
-      <c r="H10" s="102" t="s">
+      <c r="H10" s="112" t="s">
         <v>252</v>
       </c>
       <c r="I10" s="47"/>
@@ -5787,15 +5810,15 @@
       <c r="O10" s="59"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B11" s="108"/>
-      <c r="C11" s="106"/>
-      <c r="D11" s="117"/>
-      <c r="E11" s="103"/>
+      <c r="B11" s="126"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="114"/>
       <c r="F11" s="47" t="s">
         <v>281</v>
       </c>
-      <c r="G11" s="118"/>
-      <c r="H11" s="118"/>
+      <c r="G11" s="113"/>
+      <c r="H11" s="113"/>
       <c r="I11" s="47"/>
       <c r="J11" s="47" t="s">
         <v>79</v>
@@ -5807,8 +5830,8 @@
       <c r="O11" s="59"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="108"/>
-      <c r="C12" s="106"/>
+      <c r="B12" s="126"/>
+      <c r="C12" s="128"/>
       <c r="D12" s="47" t="s">
         <v>75</v>
       </c>
@@ -5818,8 +5841,8 @@
       <c r="F12" s="47" t="s">
         <v>280</v>
       </c>
-      <c r="G12" s="118"/>
-      <c r="H12" s="118"/>
+      <c r="G12" s="113"/>
+      <c r="H12" s="113"/>
       <c r="I12" s="47"/>
       <c r="J12" s="47" t="s">
         <v>157</v>
@@ -5833,19 +5856,19 @@
       <c r="O12" s="59"/>
     </row>
     <row r="13" spans="2:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="108"/>
-      <c r="C13" s="106"/>
-      <c r="D13" s="102" t="s">
+      <c r="B13" s="126"/>
+      <c r="C13" s="128"/>
+      <c r="D13" s="112" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="102" t="s">
+      <c r="E13" s="112" t="s">
         <v>73</v>
       </c>
       <c r="F13" s="47" t="s">
         <v>283</v>
       </c>
-      <c r="G13" s="118"/>
-      <c r="H13" s="118"/>
+      <c r="G13" s="113"/>
+      <c r="H13" s="113"/>
       <c r="I13" s="47"/>
       <c r="J13" s="47" t="s">
         <v>157</v>
@@ -5859,15 +5882,15 @@
       <c r="O13" s="59"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14" s="108"/>
-      <c r="C14" s="106"/>
-      <c r="D14" s="103"/>
-      <c r="E14" s="103"/>
+      <c r="B14" s="126"/>
+      <c r="C14" s="128"/>
+      <c r="D14" s="114"/>
+      <c r="E14" s="114"/>
       <c r="F14" s="72" t="s">
         <v>284</v>
       </c>
-      <c r="G14" s="118"/>
-      <c r="H14" s="118"/>
+      <c r="G14" s="113"/>
+      <c r="H14" s="113"/>
       <c r="I14" s="47"/>
       <c r="J14" s="47" t="s">
         <v>79</v>
@@ -5881,8 +5904,8 @@
       <c r="O14" s="59"/>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B15" s="108"/>
-      <c r="C15" s="107"/>
+      <c r="B15" s="126"/>
+      <c r="C15" s="129"/>
       <c r="D15" s="47" t="s">
         <v>71</v>
       </c>
@@ -5892,8 +5915,8 @@
       <c r="F15" s="47" t="s">
         <v>285</v>
       </c>
-      <c r="G15" s="103"/>
-      <c r="H15" s="103"/>
+      <c r="G15" s="114"/>
+      <c r="H15" s="114"/>
       <c r="I15" s="47"/>
       <c r="J15" s="47" t="s">
         <v>157</v>
@@ -5905,23 +5928,23 @@
       <c r="O15" s="59"/>
     </row>
     <row r="16" spans="2:15" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="108"/>
-      <c r="C16" s="104" t="s">
+      <c r="B16" s="126"/>
+      <c r="C16" s="130" t="s">
         <v>101</v>
       </c>
-      <c r="D16" s="101" t="s">
+      <c r="D16" s="133" t="s">
         <v>83</v>
       </c>
-      <c r="E16" s="119" t="s">
+      <c r="E16" s="106" t="s">
         <v>86</v>
       </c>
       <c r="F16" s="49" t="s">
         <v>286</v>
       </c>
-      <c r="G16" s="119" t="s">
+      <c r="G16" s="106" t="s">
         <v>253</v>
       </c>
-      <c r="H16" s="119" t="s">
+      <c r="H16" s="106" t="s">
         <v>254</v>
       </c>
       <c r="I16" s="49"/>
@@ -5935,15 +5958,15 @@
       <c r="O16" s="59"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B17" s="108"/>
-      <c r="C17" s="104"/>
-      <c r="D17" s="101"/>
-      <c r="E17" s="120"/>
+      <c r="B17" s="126"/>
+      <c r="C17" s="130"/>
+      <c r="D17" s="133"/>
+      <c r="E17" s="108"/>
       <c r="F17" s="70" t="s">
         <v>287</v>
       </c>
-      <c r="G17" s="128"/>
-      <c r="H17" s="128"/>
+      <c r="G17" s="107"/>
+      <c r="H17" s="107"/>
       <c r="I17" s="49"/>
       <c r="J17" s="49" t="s">
         <v>85</v>
@@ -5955,8 +5978,8 @@
       <c r="O17" s="59"/>
     </row>
     <row r="18" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B18" s="108"/>
-      <c r="C18" s="104"/>
+      <c r="B18" s="126"/>
+      <c r="C18" s="130"/>
       <c r="D18" s="49" t="s">
         <v>87</v>
       </c>
@@ -5966,8 +5989,8 @@
       <c r="F18" s="49" t="s">
         <v>288</v>
       </c>
-      <c r="G18" s="128"/>
-      <c r="H18" s="128"/>
+      <c r="G18" s="107"/>
+      <c r="H18" s="107"/>
       <c r="I18" s="49"/>
       <c r="J18" s="49"/>
       <c r="K18" s="49" t="s">
@@ -5979,8 +6002,8 @@
       <c r="O18" s="59"/>
     </row>
     <row r="19" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B19" s="108"/>
-      <c r="C19" s="104"/>
+      <c r="B19" s="126"/>
+      <c r="C19" s="130"/>
       <c r="D19" s="49" t="s">
         <v>88</v>
       </c>
@@ -5990,8 +6013,8 @@
       <c r="F19" s="49" t="s">
         <v>289</v>
       </c>
-      <c r="G19" s="128"/>
-      <c r="H19" s="128"/>
+      <c r="G19" s="107"/>
+      <c r="H19" s="107"/>
       <c r="I19" s="49"/>
       <c r="J19" s="49" t="s">
         <v>155</v>
@@ -6005,19 +6028,19 @@
       <c r="O19" s="59"/>
     </row>
     <row r="20" spans="2:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="108"/>
-      <c r="C20" s="104"/>
-      <c r="D20" s="101" t="s">
+      <c r="B20" s="126"/>
+      <c r="C20" s="130"/>
+      <c r="D20" s="133" t="s">
         <v>89</v>
       </c>
-      <c r="E20" s="119" t="s">
+      <c r="E20" s="106" t="s">
         <v>96</v>
       </c>
       <c r="F20" s="49" t="s">
         <v>290</v>
       </c>
-      <c r="G20" s="128"/>
-      <c r="H20" s="128"/>
+      <c r="G20" s="107"/>
+      <c r="H20" s="107"/>
       <c r="I20" s="49"/>
       <c r="J20" s="49" t="s">
         <v>155</v>
@@ -6031,15 +6054,15 @@
       <c r="O20" s="59"/>
     </row>
     <row r="21" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B21" s="108"/>
-      <c r="C21" s="104"/>
-      <c r="D21" s="101"/>
-      <c r="E21" s="120"/>
+      <c r="B21" s="126"/>
+      <c r="C21" s="130"/>
+      <c r="D21" s="133"/>
+      <c r="E21" s="108"/>
       <c r="F21" s="70" t="s">
         <v>291</v>
       </c>
-      <c r="G21" s="128"/>
-      <c r="H21" s="128"/>
+      <c r="G21" s="107"/>
+      <c r="H21" s="107"/>
       <c r="I21" s="49"/>
       <c r="J21" s="49" t="s">
         <v>85</v>
@@ -6051,8 +6074,8 @@
       <c r="O21" s="59"/>
     </row>
     <row r="22" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B22" s="109"/>
-      <c r="C22" s="104"/>
+      <c r="B22" s="127"/>
+      <c r="C22" s="130"/>
       <c r="D22" s="49" t="s">
         <v>90</v>
       </c>
@@ -6062,8 +6085,8 @@
       <c r="F22" s="49" t="s">
         <v>292</v>
       </c>
-      <c r="G22" s="120"/>
-      <c r="H22" s="120"/>
+      <c r="G22" s="108"/>
+      <c r="H22" s="108"/>
       <c r="I22" s="49"/>
       <c r="J22" s="49" t="s">
         <v>155</v>
@@ -6075,10 +6098,10 @@
       <c r="O22" s="59"/>
     </row>
     <row r="23" spans="2:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="104" t="s">
+      <c r="B23" s="130" t="s">
         <v>136</v>
       </c>
-      <c r="C23" s="104" t="s">
+      <c r="C23" s="130" t="s">
         <v>112</v>
       </c>
       <c r="D23" s="48" t="s">
@@ -6090,10 +6113,10 @@
       <c r="F23" s="48" t="s">
         <v>293</v>
       </c>
-      <c r="G23" s="129" t="s">
+      <c r="G23" s="109" t="s">
         <v>294</v>
       </c>
-      <c r="H23" s="129" t="s">
+      <c r="H23" s="109" t="s">
         <v>295</v>
       </c>
       <c r="I23" s="48"/>
@@ -6107,8 +6130,8 @@
       <c r="O23" s="59"/>
     </row>
     <row r="24" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B24" s="111"/>
-      <c r="C24" s="104"/>
+      <c r="B24" s="131"/>
+      <c r="C24" s="130"/>
       <c r="D24" s="48" t="s">
         <v>109</v>
       </c>
@@ -6118,8 +6141,8 @@
       <c r="F24" s="48" t="s">
         <v>296</v>
       </c>
-      <c r="G24" s="130"/>
-      <c r="H24" s="130"/>
+      <c r="G24" s="110"/>
+      <c r="H24" s="110"/>
       <c r="I24" s="48"/>
       <c r="J24" s="48" t="s">
         <v>60</v>
@@ -6133,8 +6156,8 @@
       <c r="O24" s="59"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B25" s="111"/>
-      <c r="C25" s="104"/>
+      <c r="B25" s="131"/>
+      <c r="C25" s="130"/>
       <c r="D25" s="48" t="s">
         <v>110</v>
       </c>
@@ -6144,8 +6167,8 @@
       <c r="F25" s="48" t="s">
         <v>297</v>
       </c>
-      <c r="G25" s="130"/>
-      <c r="H25" s="130"/>
+      <c r="G25" s="110"/>
+      <c r="H25" s="110"/>
       <c r="I25" s="48"/>
       <c r="J25" s="48"/>
       <c r="K25" s="48" t="s">
@@ -6157,8 +6180,8 @@
       <c r="O25" s="59"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B26" s="111"/>
-      <c r="C26" s="104"/>
+      <c r="B26" s="131"/>
+      <c r="C26" s="130"/>
       <c r="D26" s="48" t="s">
         <v>111</v>
       </c>
@@ -6168,8 +6191,8 @@
       <c r="F26" s="48" t="s">
         <v>298</v>
       </c>
-      <c r="G26" s="131"/>
-      <c r="H26" s="131"/>
+      <c r="G26" s="111"/>
+      <c r="H26" s="111"/>
       <c r="I26" s="48"/>
       <c r="J26" s="48" t="s">
         <v>156</v>
@@ -6183,8 +6206,8 @@
       <c r="O26" s="59"/>
     </row>
     <row r="27" spans="2:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="111"/>
-      <c r="C27" s="105" t="s">
+      <c r="B27" s="131"/>
+      <c r="C27" s="125" t="s">
         <v>119</v>
       </c>
       <c r="D27" s="47" t="s">
@@ -6196,10 +6219,10 @@
       <c r="F27" s="47" t="s">
         <v>299</v>
       </c>
-      <c r="G27" s="102" t="s">
+      <c r="G27" s="112" t="s">
         <v>255</v>
       </c>
-      <c r="H27" s="102" t="s">
+      <c r="H27" s="112" t="s">
         <v>256</v>
       </c>
       <c r="I27" s="47"/>
@@ -6213,8 +6236,8 @@
       <c r="O27" s="59"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B28" s="111"/>
-      <c r="C28" s="108"/>
+      <c r="B28" s="131"/>
+      <c r="C28" s="126"/>
       <c r="D28" s="47" t="s">
         <v>115</v>
       </c>
@@ -6224,8 +6247,8 @@
       <c r="F28" s="47" t="s">
         <v>300</v>
       </c>
-      <c r="G28" s="118"/>
-      <c r="H28" s="118"/>
+      <c r="G28" s="113"/>
+      <c r="H28" s="113"/>
       <c r="I28" s="47"/>
       <c r="J28" s="47"/>
       <c r="K28" s="47" t="s">
@@ -6237,8 +6260,8 @@
       <c r="O28" s="59"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B29" s="111"/>
-      <c r="C29" s="108"/>
+      <c r="B29" s="131"/>
+      <c r="C29" s="126"/>
       <c r="D29" s="47" t="s">
         <v>116</v>
       </c>
@@ -6248,8 +6271,8 @@
       <c r="F29" s="47" t="s">
         <v>301</v>
       </c>
-      <c r="G29" s="118"/>
-      <c r="H29" s="118"/>
+      <c r="G29" s="113"/>
+      <c r="H29" s="113"/>
       <c r="I29" s="47"/>
       <c r="J29" s="47" t="s">
         <v>159</v>
@@ -6261,8 +6284,8 @@
       <c r="O29" s="59"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B30" s="111"/>
-      <c r="C30" s="108"/>
+      <c r="B30" s="131"/>
+      <c r="C30" s="126"/>
       <c r="D30" s="47" t="s">
         <v>117</v>
       </c>
@@ -6272,8 +6295,8 @@
       <c r="F30" s="47" t="s">
         <v>302</v>
       </c>
-      <c r="G30" s="118"/>
-      <c r="H30" s="118"/>
+      <c r="G30" s="113"/>
+      <c r="H30" s="113"/>
       <c r="I30" s="47"/>
       <c r="J30" s="47" t="s">
         <v>160</v>
@@ -6285,9 +6308,9 @@
       <c r="O30" s="59"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B31" s="111"/>
-      <c r="C31" s="108"/>
-      <c r="D31" s="102" t="s">
+      <c r="B31" s="131"/>
+      <c r="C31" s="126"/>
+      <c r="D31" s="112" t="s">
         <v>118</v>
       </c>
       <c r="E31" s="60" t="s">
@@ -6296,8 +6319,8 @@
       <c r="F31" s="60" t="s">
         <v>303</v>
       </c>
-      <c r="G31" s="118"/>
-      <c r="H31" s="118"/>
+      <c r="G31" s="113"/>
+      <c r="H31" s="113"/>
       <c r="I31" s="60"/>
       <c r="J31" s="60"/>
       <c r="K31" s="60" t="s">
@@ -6309,17 +6332,17 @@
       <c r="O31" s="59"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B32" s="111"/>
-      <c r="C32" s="109"/>
-      <c r="D32" s="103"/>
+      <c r="B32" s="131"/>
+      <c r="C32" s="127"/>
+      <c r="D32" s="114"/>
       <c r="E32" s="60" t="s">
         <v>134</v>
       </c>
       <c r="F32" s="60" t="s">
         <v>304</v>
       </c>
-      <c r="G32" s="103"/>
-      <c r="H32" s="103"/>
+      <c r="G32" s="114"/>
+      <c r="H32" s="114"/>
       <c r="I32" s="60"/>
       <c r="J32" s="60" t="s">
         <v>131</v>
@@ -6333,25 +6356,25 @@
       <c r="O32" s="59"/>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B33" s="104" t="s">
+      <c r="B33" s="130" t="s">
         <v>151</v>
       </c>
-      <c r="C33" s="104" t="s">
+      <c r="C33" s="130" t="s">
         <v>150</v>
       </c>
-      <c r="D33" s="110" t="s">
+      <c r="D33" s="124" t="s">
         <v>137</v>
       </c>
-      <c r="E33" s="112" t="s">
+      <c r="E33" s="103" t="s">
         <v>141</v>
       </c>
       <c r="F33" s="50" t="s">
         <v>305</v>
       </c>
-      <c r="G33" s="124" t="s">
+      <c r="G33" s="121" t="s">
         <v>257</v>
       </c>
-      <c r="H33" s="110" t="s">
+      <c r="H33" s="124" t="s">
         <v>258</v>
       </c>
       <c r="I33" s="51"/>
@@ -6365,15 +6388,15 @@
       <c r="O33" s="59"/>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B34" s="111"/>
-      <c r="C34" s="111"/>
-      <c r="D34" s="110"/>
-      <c r="E34" s="113"/>
+      <c r="B34" s="131"/>
+      <c r="C34" s="131"/>
+      <c r="D34" s="124"/>
+      <c r="E34" s="105"/>
       <c r="F34" s="50" t="s">
         <v>306</v>
       </c>
-      <c r="G34" s="125"/>
-      <c r="H34" s="110"/>
+      <c r="G34" s="122"/>
+      <c r="H34" s="124"/>
       <c r="I34" s="66"/>
       <c r="J34" s="50" t="s">
         <v>152</v>
@@ -6385,8 +6408,8 @@
       <c r="O34" s="59"/>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B35" s="111"/>
-      <c r="C35" s="111"/>
+      <c r="B35" s="131"/>
+      <c r="C35" s="131"/>
       <c r="D35" s="50" t="s">
         <v>138</v>
       </c>
@@ -6396,8 +6419,8 @@
       <c r="F35" s="50" t="s">
         <v>307</v>
       </c>
-      <c r="G35" s="125"/>
-      <c r="H35" s="110"/>
+      <c r="G35" s="122"/>
+      <c r="H35" s="124"/>
       <c r="I35" s="66"/>
       <c r="J35" s="50"/>
       <c r="K35" s="50" t="s">
@@ -6409,8 +6432,8 @@
       <c r="O35" s="59"/>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B36" s="111"/>
-      <c r="C36" s="111"/>
+      <c r="B36" s="131"/>
+      <c r="C36" s="131"/>
       <c r="D36" s="50" t="s">
         <v>139</v>
       </c>
@@ -6420,8 +6443,8 @@
       <c r="F36" s="50" t="s">
         <v>308</v>
       </c>
-      <c r="G36" s="125"/>
-      <c r="H36" s="110"/>
+      <c r="G36" s="122"/>
+      <c r="H36" s="124"/>
       <c r="I36" s="66"/>
       <c r="J36" s="50" t="s">
         <v>161</v>
@@ -6435,19 +6458,19 @@
       <c r="O36" s="59"/>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B37" s="111"/>
-      <c r="C37" s="111"/>
+      <c r="B37" s="131"/>
+      <c r="C37" s="131"/>
       <c r="D37" s="50" t="s">
         <v>140</v>
       </c>
-      <c r="E37" s="112" t="s">
+      <c r="E37" s="103" t="s">
         <v>148</v>
       </c>
       <c r="F37" s="50" t="s">
         <v>309</v>
       </c>
-      <c r="G37" s="125"/>
-      <c r="H37" s="110"/>
+      <c r="G37" s="122"/>
+      <c r="H37" s="124"/>
       <c r="I37" s="66"/>
       <c r="J37" s="50"/>
       <c r="K37" s="50" t="s">
@@ -6459,15 +6482,15 @@
       <c r="O37" s="59"/>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B38" s="111"/>
-      <c r="C38" s="111"/>
+      <c r="B38" s="131"/>
+      <c r="C38" s="131"/>
       <c r="D38" s="50"/>
-      <c r="E38" s="113"/>
+      <c r="E38" s="105"/>
       <c r="F38" s="50" t="s">
         <v>310</v>
       </c>
-      <c r="G38" s="125"/>
-      <c r="H38" s="110"/>
+      <c r="G38" s="122"/>
+      <c r="H38" s="124"/>
       <c r="I38" s="66"/>
       <c r="J38" s="50" t="s">
         <v>152</v>
@@ -6479,8 +6502,8 @@
       <c r="O38" s="59"/>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B39" s="111"/>
-      <c r="C39" s="111"/>
+      <c r="B39" s="131"/>
+      <c r="C39" s="131"/>
       <c r="D39" s="50" t="s">
         <v>144</v>
       </c>
@@ -6490,8 +6513,8 @@
       <c r="F39" s="50" t="s">
         <v>311</v>
       </c>
-      <c r="G39" s="125"/>
-      <c r="H39" s="110"/>
+      <c r="G39" s="122"/>
+      <c r="H39" s="124"/>
       <c r="I39" s="66"/>
       <c r="J39" s="50" t="s">
         <v>161</v>
@@ -6503,19 +6526,19 @@
       <c r="O39" s="59"/>
     </row>
     <row r="40" spans="2:15" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="111"/>
-      <c r="C40" s="111"/>
-      <c r="D40" s="112" t="s">
+      <c r="B40" s="131"/>
+      <c r="C40" s="131"/>
+      <c r="D40" s="103" t="s">
         <v>145</v>
       </c>
-      <c r="E40" s="112" t="s">
+      <c r="E40" s="103" t="s">
         <v>146</v>
       </c>
       <c r="F40" s="50" t="s">
         <v>312</v>
       </c>
-      <c r="G40" s="125"/>
-      <c r="H40" s="110"/>
+      <c r="G40" s="122"/>
+      <c r="H40" s="124"/>
       <c r="I40" s="66"/>
       <c r="J40" s="50" t="s">
         <v>152</v>
@@ -6529,15 +6552,15 @@
       <c r="O40" s="59"/>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B41" s="111"/>
-      <c r="C41" s="111"/>
-      <c r="D41" s="113"/>
-      <c r="E41" s="113"/>
+      <c r="B41" s="131"/>
+      <c r="C41" s="131"/>
+      <c r="D41" s="105"/>
+      <c r="E41" s="105"/>
       <c r="F41" s="71" t="s">
         <v>312</v>
       </c>
-      <c r="G41" s="126"/>
-      <c r="H41" s="110"/>
+      <c r="G41" s="123"/>
+      <c r="H41" s="124"/>
       <c r="I41" s="66"/>
       <c r="J41" s="50" t="s">
         <v>152</v>
@@ -6549,8 +6572,8 @@
       <c r="O41" s="59"/>
     </row>
     <row r="42" spans="2:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="111"/>
-      <c r="C42" s="104" t="s">
+      <c r="B42" s="131"/>
+      <c r="C42" s="130" t="s">
         <v>120</v>
       </c>
       <c r="D42" s="50" t="s">
@@ -6562,10 +6585,10 @@
       <c r="F42" s="50" t="s">
         <v>313</v>
       </c>
-      <c r="G42" s="112" t="s">
+      <c r="G42" s="103" t="s">
         <v>251</v>
       </c>
-      <c r="H42" s="112" t="s">
+      <c r="H42" s="103" t="s">
         <v>252</v>
       </c>
       <c r="I42" s="50"/>
@@ -6581,8 +6604,8 @@
       <c r="O42" s="59"/>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B43" s="111"/>
-      <c r="C43" s="104"/>
+      <c r="B43" s="131"/>
+      <c r="C43" s="130"/>
       <c r="D43" s="50" t="s">
         <v>74</v>
       </c>
@@ -6592,8 +6615,8 @@
       <c r="F43" s="50" t="s">
         <v>314</v>
       </c>
-      <c r="G43" s="127"/>
-      <c r="H43" s="127"/>
+      <c r="G43" s="104"/>
+      <c r="H43" s="104"/>
       <c r="I43" s="50"/>
       <c r="J43" s="50"/>
       <c r="K43" s="50" t="s">
@@ -6605,8 +6628,8 @@
       <c r="O43" s="59"/>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B44" s="111"/>
-      <c r="C44" s="104"/>
+      <c r="B44" s="131"/>
+      <c r="C44" s="130"/>
       <c r="D44" s="50" t="s">
         <v>122</v>
       </c>
@@ -6616,8 +6639,8 @@
       <c r="F44" s="50" t="s">
         <v>315</v>
       </c>
-      <c r="G44" s="113"/>
-      <c r="H44" s="113"/>
+      <c r="G44" s="105"/>
+      <c r="H44" s="105"/>
       <c r="I44" s="50"/>
       <c r="J44" s="50" t="s">
         <v>81</v>
@@ -6664,14 +6687,27 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="G42:G44"/>
-    <mergeCell ref="H42:H44"/>
-    <mergeCell ref="G16:G22"/>
-    <mergeCell ref="H16:H22"/>
-    <mergeCell ref="G23:G26"/>
-    <mergeCell ref="H23:H26"/>
-    <mergeCell ref="G27:G32"/>
-    <mergeCell ref="H27:H32"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C16:C22"/>
+    <mergeCell ref="C10:C15"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="C3:C9"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="C33:C41"/>
+    <mergeCell ref="B33:B44"/>
+    <mergeCell ref="D40:D41"/>
+    <mergeCell ref="B10:B22"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="B23:B32"/>
+    <mergeCell ref="C23:C26"/>
+    <mergeCell ref="C42:C44"/>
+    <mergeCell ref="D10:D11"/>
     <mergeCell ref="G3:G9"/>
     <mergeCell ref="H3:H9"/>
     <mergeCell ref="G10:G15"/>
@@ -6688,27 +6724,14 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="G33:G41"/>
     <mergeCell ref="H33:H41"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="C3:C9"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="C33:C41"/>
-    <mergeCell ref="B33:B44"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="B10:B22"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="B23:B32"/>
-    <mergeCell ref="C23:C26"/>
-    <mergeCell ref="C42:C44"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="C16:C22"/>
-    <mergeCell ref="C10:C15"/>
-    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="G42:G44"/>
+    <mergeCell ref="H42:H44"/>
+    <mergeCell ref="G16:G22"/>
+    <mergeCell ref="H16:H22"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="H23:H26"/>
+    <mergeCell ref="G27:G32"/>
+    <mergeCell ref="H27:H32"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6767,22 +6790,22 @@
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="133" t="s">
+      <c r="B3" s="144" t="s">
         <v>196</v>
       </c>
-      <c r="C3" s="132" t="s">
+      <c r="C3" s="143" t="s">
         <v>195</v>
       </c>
-      <c r="D3" s="132" t="s">
+      <c r="D3" s="143" t="s">
         <v>187</v>
       </c>
       <c r="E3" s="61" t="s">
         <v>272</v>
       </c>
-      <c r="F3" s="132" t="s">
+      <c r="F3" s="143" t="s">
         <v>202</v>
       </c>
-      <c r="G3" s="132" t="s">
+      <c r="G3" s="143" t="s">
         <v>203</v>
       </c>
       <c r="H3" s="61" t="s">
@@ -6793,14 +6816,14 @@
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="133"/>
-      <c r="C4" s="132"/>
-      <c r="D4" s="132"/>
+      <c r="B4" s="144"/>
+      <c r="C4" s="143"/>
+      <c r="D4" s="143"/>
       <c r="E4" s="73" t="s">
         <v>276</v>
       </c>
-      <c r="F4" s="132"/>
-      <c r="G4" s="132"/>
+      <c r="F4" s="143"/>
+      <c r="G4" s="143"/>
       <c r="H4" s="61" t="s">
         <v>206</v>
       </c>
@@ -6809,30 +6832,30 @@
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="133"/>
-      <c r="C5" s="132"/>
-      <c r="D5" s="132" t="s">
+      <c r="B5" s="144"/>
+      <c r="C5" s="143"/>
+      <c r="D5" s="143" t="s">
         <v>188</v>
       </c>
       <c r="E5" s="73" t="s">
         <v>317</v>
       </c>
-      <c r="F5" s="132"/>
-      <c r="G5" s="132"/>
+      <c r="F5" s="143"/>
+      <c r="G5" s="143"/>
       <c r="H5" s="61"/>
       <c r="I5" s="61" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="133"/>
-      <c r="C6" s="132"/>
-      <c r="D6" s="132"/>
+      <c r="B6" s="144"/>
+      <c r="C6" s="143"/>
+      <c r="D6" s="143"/>
       <c r="E6" s="61" t="s">
         <v>316</v>
       </c>
-      <c r="F6" s="132"/>
-      <c r="G6" s="132"/>
+      <c r="F6" s="143"/>
+      <c r="G6" s="143"/>
       <c r="H6" s="61" t="s">
         <v>208</v>
       </c>
@@ -6841,30 +6864,30 @@
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="133"/>
-      <c r="C7" s="132"/>
-      <c r="D7" s="132" t="s">
+      <c r="B7" s="144"/>
+      <c r="C7" s="143"/>
+      <c r="D7" s="143" t="s">
         <v>189</v>
       </c>
       <c r="E7" s="61" t="s">
         <v>318</v>
       </c>
-      <c r="F7" s="132"/>
-      <c r="G7" s="132"/>
+      <c r="F7" s="143"/>
+      <c r="G7" s="143"/>
       <c r="H7" s="61"/>
       <c r="I7" s="61" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="133"/>
-      <c r="C8" s="132"/>
-      <c r="D8" s="132"/>
+      <c r="B8" s="144"/>
+      <c r="C8" s="143"/>
+      <c r="D8" s="143"/>
       <c r="E8" s="61" t="s">
         <v>318</v>
       </c>
-      <c r="F8" s="132"/>
-      <c r="G8" s="132"/>
+      <c r="F8" s="143"/>
+      <c r="G8" s="143"/>
       <c r="H8" s="61" t="s">
         <v>209</v>
       </c>
@@ -6873,30 +6896,30 @@
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="133"/>
-      <c r="C9" s="132"/>
-      <c r="D9" s="132" t="s">
+      <c r="B9" s="144"/>
+      <c r="C9" s="143"/>
+      <c r="D9" s="143" t="s">
         <v>190</v>
       </c>
       <c r="E9" s="61" t="s">
         <v>319</v>
       </c>
-      <c r="F9" s="132"/>
-      <c r="G9" s="132"/>
+      <c r="F9" s="143"/>
+      <c r="G9" s="143"/>
       <c r="H9" s="61"/>
       <c r="I9" s="61" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="133"/>
-      <c r="C10" s="132"/>
-      <c r="D10" s="132"/>
+      <c r="B10" s="144"/>
+      <c r="C10" s="143"/>
+      <c r="D10" s="143"/>
       <c r="E10" s="61" t="s">
         <v>320</v>
       </c>
-      <c r="F10" s="132"/>
-      <c r="G10" s="132"/>
+      <c r="F10" s="143"/>
+      <c r="G10" s="143"/>
       <c r="H10" s="61" t="s">
         <v>210</v>
       </c>
@@ -6905,7 +6928,7 @@
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="133"/>
+      <c r="B11" s="144"/>
       <c r="C11" s="61" t="s">
         <v>194</v>
       </c>
@@ -6929,7 +6952,7 @@
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="133"/>
+      <c r="B12" s="144"/>
       <c r="C12" s="61" t="s">
         <v>193</v>
       </c>
@@ -6992,10 +7015,10 @@
       <c r="B15" s="138" t="s">
         <v>234</v>
       </c>
-      <c r="C15" s="132" t="s">
+      <c r="C15" s="143" t="s">
         <v>195</v>
       </c>
-      <c r="D15" s="132" t="s">
+      <c r="D15" s="143" t="s">
         <v>188</v>
       </c>
       <c r="E15" s="61" t="s">
@@ -7014,8 +7037,8 @@
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="138"/>
-      <c r="C16" s="132"/>
-      <c r="D16" s="132"/>
+      <c r="C16" s="143"/>
+      <c r="D16" s="143"/>
       <c r="E16" s="61" t="s">
         <v>322</v>
       </c>
@@ -7030,7 +7053,7 @@
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="138"/>
-      <c r="C17" s="132"/>
+      <c r="C17" s="143"/>
       <c r="D17" s="61" t="s">
         <v>225</v>
       </c>
@@ -7046,7 +7069,7 @@
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="138"/>
-      <c r="C18" s="132"/>
+      <c r="C18" s="143"/>
       <c r="D18" s="61" t="s">
         <v>242</v>
       </c>
@@ -7064,7 +7087,7 @@
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="138"/>
-      <c r="C19" s="132"/>
+      <c r="C19" s="143"/>
       <c r="D19" s="61" t="s">
         <v>226</v>
       </c>
@@ -7239,10 +7262,10 @@
       <c r="B31" s="142" t="s">
         <v>259</v>
       </c>
-      <c r="C31" s="132" t="s">
+      <c r="C31" s="143" t="s">
         <v>195</v>
       </c>
-      <c r="D31" s="132" t="s">
+      <c r="D31" s="143" t="s">
         <v>188</v>
       </c>
       <c r="E31" s="61" t="s">
@@ -7259,8 +7282,8 @@
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32" s="142"/>
-      <c r="C32" s="132"/>
-      <c r="D32" s="132"/>
+      <c r="C32" s="143"/>
+      <c r="D32" s="143"/>
       <c r="E32" s="61" t="s">
         <v>338</v>
       </c>
@@ -7271,7 +7294,7 @@
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="142"/>
-      <c r="C33" s="132"/>
+      <c r="C33" s="143"/>
       <c r="D33" s="61" t="s">
         <v>225</v>
       </c>
@@ -7285,7 +7308,7 @@
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="142"/>
-      <c r="C34" s="132"/>
+      <c r="C34" s="143"/>
       <c r="D34" s="61"/>
       <c r="E34" s="61"/>
       <c r="F34" s="140"/>
@@ -7295,7 +7318,7 @@
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="142"/>
-      <c r="C35" s="132"/>
+      <c r="C35" s="143"/>
       <c r="D35" s="61"/>
       <c r="E35" s="61"/>
       <c r="F35" s="141"/>
@@ -7395,11 +7418,21 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="D36:D37"/>
-    <mergeCell ref="F36:F39"/>
+    <mergeCell ref="C3:C10"/>
+    <mergeCell ref="B3:B12"/>
+    <mergeCell ref="F3:F10"/>
+    <mergeCell ref="G3:G10"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="C20:C23"/>
     <mergeCell ref="G36:G39"/>
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="C40:C42"/>
@@ -7416,21 +7449,11 @@
     <mergeCell ref="G31:G35"/>
     <mergeCell ref="C15:C19"/>
     <mergeCell ref="D20:D21"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="C20:C23"/>
-    <mergeCell ref="C3:C10"/>
-    <mergeCell ref="B3:B12"/>
-    <mergeCell ref="F3:F10"/>
-    <mergeCell ref="G3:G10"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="F36:F39"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7440,70 +7463,86 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D6"/>
+  <dimension ref="B1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.375" customWidth="1"/>
-    <col min="2" max="2" width="59.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.25" customWidth="1"/>
+    <col min="3" max="3" width="44" customWidth="1"/>
+    <col min="4" max="4" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:6" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="74" t="s">
         <v>341</v>
       </c>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="78" t="s">
         <v>342</v>
       </c>
-      <c r="D2" s="75" t="s">
+      <c r="D2" s="81" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="75" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="76" t="s">
+      <c r="C3" s="78" t="s">
+        <v>354</v>
+      </c>
+      <c r="D3" s="81"/>
+      <c r="E3" t="s">
+        <v>347</v>
+      </c>
+      <c r="F3" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="76" t="s">
+        <v>344</v>
+      </c>
+      <c r="C4" s="79" t="s">
+        <v>348</v>
+      </c>
+      <c r="D4" s="81">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="75" t="s">
         <v>345</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="77" t="s">
-        <v>347</v>
-      </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76" t="s">
+      <c r="C5" s="80" t="s">
+        <v>349</v>
+      </c>
+      <c r="D5" s="81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="77" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="76" t="s">
-        <v>349</v>
-      </c>
-      <c r="C5" s="76"/>
-      <c r="D5" s="78" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="79" t="s">
-        <v>351</v>
-      </c>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78" t="s">
-        <v>350</v>
+      <c r="C6" s="80" t="s">
+        <v>352</v>
+      </c>
+      <c r="D6" s="81">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>